<commit_message>
Update spec to V0.2
</commit_message>
<xml_diff>
--- a/DOC/register map.xlsx
+++ b/DOC/register map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="227">
   <si>
     <t>Offset</t>
   </si>
@@ -261,48 +261,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>HDD 12V/6V Power Enable</t>
-  </si>
-  <si>
-    <t>HDD 12V/7V Power Enable</t>
-  </si>
-  <si>
-    <t>HDD 12V/8V Power Enable</t>
-  </si>
-  <si>
-    <t>HDD 12V/9V Power Enable</t>
-  </si>
-  <si>
-    <t>HDD 12V/10V Power Enable</t>
-  </si>
-  <si>
-    <t>HDD 12V/11V Power Enable</t>
-  </si>
-  <si>
-    <t>HDD 12V/12V Power Enable</t>
-  </si>
-  <si>
-    <t>HDD 12V/13V Power Enable</t>
-  </si>
-  <si>
-    <t>HDD 12V/14V Power Enable</t>
-  </si>
-  <si>
-    <t>HDD 12V/15V Power Enable</t>
-  </si>
-  <si>
-    <t>HDD 12V/16V Power Enable</t>
-  </si>
-  <si>
-    <t>HDD 12V/17V Power Enable</t>
-  </si>
-  <si>
-    <t>HDD 12V/18V Power Enable</t>
-  </si>
-  <si>
-    <t>HDD 12V/19V Power Enable</t>
-  </si>
-  <si>
     <t>Field</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -332,39 +290,10 @@
     <t>bit7</t>
   </si>
   <si>
-    <t>bit8</t>
-  </si>
-  <si>
-    <t>bit9</t>
-  </si>
-  <si>
-    <t>bit10</t>
-  </si>
-  <si>
-    <t>bit11</t>
-  </si>
-  <si>
-    <t>bit12</t>
-  </si>
-  <si>
-    <t>bit13</t>
-  </si>
-  <si>
-    <t>bit14</t>
-  </si>
-  <si>
     <t>00h</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>01h</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>02h</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>10h</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -428,53 +357,6 @@
   </si>
   <si>
     <t>20h</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>21h</t>
-  </si>
-  <si>
-    <t>22h</t>
-  </si>
-  <si>
-    <t>23h</t>
-  </si>
-  <si>
-    <t>24h</t>
-  </si>
-  <si>
-    <t>25h</t>
-  </si>
-  <si>
-    <t>26h</t>
-  </si>
-  <si>
-    <t>27h</t>
-  </si>
-  <si>
-    <t>28h</t>
-  </si>
-  <si>
-    <t>29h</t>
-  </si>
-  <si>
-    <t>2Ah</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2Bh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2Ch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2Dh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2Eh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -537,9 +419,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>31h</t>
-  </si>
-  <si>
     <t>32h</t>
   </si>
   <si>
@@ -553,35 +432,6 @@
   </si>
   <si>
     <t>36h</t>
-  </si>
-  <si>
-    <t>37h</t>
-  </si>
-  <si>
-    <t>38h</t>
-  </si>
-  <si>
-    <t>39h</t>
-  </si>
-  <si>
-    <t>3Ah</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3Bh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3Ch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3Dh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3Eh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>H: Drive Failure;
@@ -653,11 +503,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>L: An event has occurred that requires interrupt service;
-H: no interrupt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>L: MiniSAS HD Module power enable for device management</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -749,12 +594,6 @@
   <si>
     <t>H: Loss of SAS links (x1 ~x3)
 L: No SAS links or SAS links (x4) health</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>L: Reserved
-PWM: Reserved
-H: Any failure in whole enclosure;</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -799,6 +638,208 @@
   </si>
   <si>
     <t>bit7-4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>11h</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDD 12V/5V Power Enable</t>
+  </si>
+  <si>
+    <t>HDD 12V/5V Power Enable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01h</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>02h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>03h</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>05h</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>04h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>21h</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>22h</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>23h</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>24h</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>25h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>26h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>27h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>31h</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>37h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>90h</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bit0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDD Insert Interrupt</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P5V_GD_HDD Interrupt</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P12V_GD_HDD Interrupt</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>L: Reserved
+PWM: Reserved
+H: Any failure in whole enclosure</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>L: An event has occurred that requires interrupt service
+H: no interrupt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L: An event has occurred that requires interrupt service
+H: no interrupt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L: MiniSAS HD cable module insert; H: No Inserted</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H: Some HDD have been inserted or unpluged
+This bit will be reset after I2C read</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>H: Some 5V Power good signal have been changed
+This bit will be reset after I2C read</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>H: Some 12V Power good signal have been changed
+This bit will be reset after I2C read</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>F0h</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bit7</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reserved</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bit7</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reserved</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bit6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reserved</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bit7-0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPLD_MAJ_VER</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>F1h</t>
+  </si>
+  <si>
+    <t>F2h</t>
+  </si>
+  <si>
+    <t>CPLD_MIN_VER</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPLD_HDR_CHK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bit&lt;7:0&gt; CPLD Minor Version Number Register
+Identifies the minor revision of the Baseboard CPLD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPLD Major Version Number Register
+Identifies the major revision of the Baseboard CPLD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPLD Header Information Checksum Register</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -852,7 +893,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -867,6 +908,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1154,10 +1201,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F119"/>
+  <dimension ref="A1:F130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="E120" sqref="E120"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="E131" sqref="E131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1166,7 +1213,7 @@
     <col min="2" max="2" width="7.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="30.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="63.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62.75" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
@@ -1176,7 +1223,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -1192,11 +1239,11 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
-        <v>103</v>
+      <c r="A2" s="8" t="s">
+        <v>82</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -1209,9 +1256,9 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="6"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
@@ -1224,9 +1271,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="6"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="1" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
@@ -1239,9 +1286,9 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="6"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="1" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
@@ -1254,9 +1301,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="6"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="1" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
@@ -1269,9 +1316,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="6"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="1" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
@@ -1284,9 +1331,9 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" s="6"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>9</v>
@@ -1299,9 +1346,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9" s="6"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="1" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>10</v>
@@ -1314,9 +1361,11 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="6"/>
-      <c r="B10" s="1" t="s">
-        <v>96</v>
+      <c r="A10" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>11</v>
@@ -1329,9 +1378,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="6"/>
-      <c r="B11" s="1" t="s">
-        <v>97</v>
+      <c r="A11" s="8"/>
+      <c r="B11" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>12</v>
@@ -1344,9 +1393,9 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="6"/>
-      <c r="B12" s="1" t="s">
-        <v>98</v>
+      <c r="A12" s="8"/>
+      <c r="B12" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
@@ -1359,9 +1408,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="6"/>
-      <c r="B13" s="1" t="s">
-        <v>99</v>
+      <c r="A13" s="8"/>
+      <c r="B13" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>14</v>
@@ -1374,9 +1423,9 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="6"/>
-      <c r="B14" s="1" t="s">
-        <v>100</v>
+      <c r="A14" s="8"/>
+      <c r="B14" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>15</v>
@@ -1389,9 +1438,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="6"/>
-      <c r="B15" s="1" t="s">
-        <v>101</v>
+      <c r="A15" s="8"/>
+      <c r="B15" s="7" t="s">
+        <v>79</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>16</v>
@@ -1403,10 +1452,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A16" s="6"/>
-      <c r="B16" s="1" t="s">
-        <v>102</v>
+    <row r="16" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="8"/>
+      <c r="B16" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>17</v>
@@ -1419,18 +1468,23 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="6" t="s">
-        <v>104</v>
+      <c r="A18" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>22</v>
@@ -1443,9 +1497,9 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="6"/>
+      <c r="A19" s="8"/>
       <c r="B19" s="1" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>23</v>
@@ -1458,9 +1512,9 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="6"/>
+      <c r="A20" s="8"/>
       <c r="B20" s="1" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>24</v>
@@ -1473,9 +1527,9 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="6"/>
+      <c r="A21" s="8"/>
       <c r="B21" s="1" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>25</v>
@@ -1488,9 +1542,9 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="6"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="1" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>26</v>
@@ -1503,9 +1557,9 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="6"/>
+      <c r="A23" s="8"/>
       <c r="B23" s="1" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>27</v>
@@ -1518,9 +1572,9 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="6"/>
+      <c r="A24" s="8"/>
       <c r="B24" s="1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>28</v>
@@ -1533,9 +1587,9 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="6"/>
+      <c r="A25" s="8"/>
       <c r="B25" s="1" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>29</v>
@@ -1548,9 +1602,11 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="6"/>
-      <c r="B26" s="1" t="s">
-        <v>96</v>
+      <c r="A26" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>30</v>
@@ -1563,9 +1619,9 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="6"/>
-      <c r="B27" s="1" t="s">
-        <v>97</v>
+      <c r="A27" s="8"/>
+      <c r="B27" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>31</v>
@@ -1578,9 +1634,9 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="6"/>
-      <c r="B28" s="1" t="s">
-        <v>98</v>
+      <c r="A28" s="8"/>
+      <c r="B28" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>32</v>
@@ -1593,9 +1649,9 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="6"/>
-      <c r="B29" s="1" t="s">
-        <v>99</v>
+      <c r="A29" s="8"/>
+      <c r="B29" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>33</v>
@@ -1608,9 +1664,9 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="6"/>
-      <c r="B30" s="1" t="s">
-        <v>100</v>
+      <c r="A30" s="8"/>
+      <c r="B30" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>34</v>
@@ -1623,9 +1679,9 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="6"/>
-      <c r="B31" s="1" t="s">
-        <v>101</v>
+      <c r="A31" s="8"/>
+      <c r="B31" s="7" t="s">
+        <v>79</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>35</v>
@@ -1637,10 +1693,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32" s="6"/>
-      <c r="B32" s="1" t="s">
-        <v>102</v>
+    <row r="32" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="8"/>
+      <c r="B32" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>36</v>
@@ -1653,18 +1709,23 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
+      <c r="A33" s="8"/>
+      <c r="B33" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" s="6" t="s">
-        <v>105</v>
+      <c r="A34" s="8" t="s">
+        <v>185</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>40</v>
@@ -1677,9 +1738,9 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" s="6"/>
+      <c r="A35" s="8"/>
       <c r="B35" s="1" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>41</v>
@@ -1692,9 +1753,9 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="6"/>
+      <c r="A36" s="8"/>
       <c r="B36" s="1" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>42</v>
@@ -1707,9 +1768,9 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="6"/>
+      <c r="A37" s="8"/>
       <c r="B37" s="1" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>43</v>
@@ -1722,9 +1783,9 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="6"/>
+      <c r="A38" s="8"/>
       <c r="B38" s="1" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>44</v>
@@ -1737,9 +1798,9 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" s="6"/>
+      <c r="A39" s="8"/>
       <c r="B39" s="1" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>45</v>
@@ -1752,9 +1813,9 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" s="6"/>
+      <c r="A40" s="8"/>
       <c r="B40" s="1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>46</v>
@@ -1767,9 +1828,9 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="6"/>
+      <c r="A41" s="8"/>
       <c r="B41" s="1" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>47</v>
@@ -1782,9 +1843,11 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="6"/>
-      <c r="B42" s="1" t="s">
-        <v>96</v>
+      <c r="A42" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>48</v>
@@ -1797,9 +1860,9 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="6"/>
-      <c r="B43" s="1" t="s">
-        <v>97</v>
+      <c r="A43" s="8"/>
+      <c r="B43" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>49</v>
@@ -1812,9 +1875,9 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="6"/>
-      <c r="B44" s="1" t="s">
-        <v>98</v>
+      <c r="A44" s="8"/>
+      <c r="B44" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>50</v>
@@ -1827,9 +1890,9 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="6"/>
-      <c r="B45" s="1" t="s">
-        <v>99</v>
+      <c r="A45" s="8"/>
+      <c r="B45" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>51</v>
@@ -1842,9 +1905,9 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="6"/>
-      <c r="B46" s="1" t="s">
-        <v>100</v>
+      <c r="A46" s="8"/>
+      <c r="B46" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>52</v>
@@ -1857,9 +1920,9 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" s="6"/>
-      <c r="B47" s="1" t="s">
-        <v>101</v>
+      <c r="A47" s="8"/>
+      <c r="B47" s="7" t="s">
+        <v>79</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>53</v>
@@ -1871,10 +1934,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A48" s="6"/>
-      <c r="B48" s="1" t="s">
-        <v>102</v>
+    <row r="48" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="8"/>
+      <c r="B48" s="7" t="s">
+        <v>215</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>54</v>
@@ -1887,1270 +1950,1413 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
+      <c r="A49" s="8"/>
+      <c r="B49" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="D49" s="7"/>
+      <c r="E49" s="2" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A50" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>221</v>
-      </c>
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A51" s="6"/>
+      <c r="A51" s="8" t="s">
+        <v>83</v>
+      </c>
       <c r="B51" s="1" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>222</v>
+        <v>173</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A52" s="6"/>
+      <c r="A52" s="8"/>
       <c r="B52" s="1" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>216</v>
+        <v>180</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A53" s="6"/>
+      <c r="A53" s="8"/>
       <c r="B53" s="1" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>75</v>
+        <v>179</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A54" s="6"/>
+      <c r="A54" s="8"/>
       <c r="B54" s="1" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>76</v>
+        <v>179</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A55" s="6"/>
+      <c r="A55" s="8"/>
       <c r="B55" s="1" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>77</v>
+        <v>179</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A56" s="6"/>
+      <c r="A56" s="8"/>
       <c r="B56" s="1" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>78</v>
+        <v>179</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A57" s="6"/>
+      <c r="A57" s="8"/>
       <c r="B57" s="1" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>79</v>
+        <v>179</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A58" s="6"/>
+      <c r="A58" s="8"/>
       <c r="B58" s="1" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>80</v>
+        <v>179</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A59" s="6"/>
-      <c r="B59" s="1" t="s">
-        <v>97</v>
+      <c r="A59" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>81</v>
+        <v>179</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A60" s="6"/>
-      <c r="B60" s="1" t="s">
-        <v>98</v>
+      <c r="A60" s="8"/>
+      <c r="B60" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>82</v>
+        <v>179</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A61" s="6"/>
-      <c r="B61" s="1" t="s">
-        <v>99</v>
+      <c r="A61" s="8"/>
+      <c r="B61" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>83</v>
+        <v>179</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A62" s="6"/>
-      <c r="B62" s="1" t="s">
-        <v>100</v>
+      <c r="A62" s="8"/>
+      <c r="B62" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>84</v>
+        <v>179</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A63" s="6"/>
-      <c r="B63" s="1" t="s">
-        <v>101</v>
+      <c r="A63" s="8"/>
+      <c r="B63" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>85</v>
+        <v>179</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A64" s="6"/>
-      <c r="B64" s="1" t="s">
-        <v>102</v>
+      <c r="A64" s="8"/>
+      <c r="B64" s="7" t="s">
+        <v>79</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>86</v>
+        <v>179</v>
       </c>
       <c r="F64" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A65" s="8"/>
+      <c r="B65" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A66" s="8"/>
+      <c r="B66" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="D66" s="7"/>
+      <c r="E66" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F66" s="7" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A65" s="6"/>
-      <c r="B65" s="6"/>
-      <c r="C65" s="6"/>
-      <c r="D65" s="6"/>
-      <c r="E65" s="6"/>
-    </row>
-    <row r="66" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A66" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A67" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>219</v>
-      </c>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A67" s="8"/>
+      <c r="B67" s="8"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8"/>
+      <c r="F67" s="8"/>
     </row>
     <row r="68" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A68" s="1" t="s">
-        <v>127</v>
+      <c r="A68" s="8" t="s">
+        <v>102</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>217</v>
+        <v>103</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A69" s="1" t="s">
-        <v>128</v>
-      </c>
+      <c r="A69" s="8"/>
       <c r="B69" s="1" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>217</v>
+        <v>103</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A70" s="1" t="s">
-        <v>129</v>
+      <c r="A70" s="8" t="s">
+        <v>186</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>140</v>
+        <v>103</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>217</v>
+        <v>169</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A71" s="1" t="s">
-        <v>130</v>
-      </c>
+      <c r="A71" s="8"/>
       <c r="B71" s="1" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>140</v>
+        <v>103</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>217</v>
+        <v>169</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A72" s="1" t="s">
-        <v>131</v>
+      <c r="A72" s="8" t="s">
+        <v>187</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>140</v>
+        <v>103</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>217</v>
+        <v>169</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A73" s="1" t="s">
-        <v>132</v>
-      </c>
+      <c r="A73" s="8"/>
       <c r="B73" s="1" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>140</v>
+        <v>103</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>217</v>
+        <v>169</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A74" s="1" t="s">
-        <v>133</v>
+      <c r="A74" s="8" t="s">
+        <v>188</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>140</v>
+        <v>103</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>217</v>
+        <v>169</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A75" s="1" t="s">
-        <v>134</v>
-      </c>
+      <c r="A75" s="8"/>
       <c r="B75" s="1" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>140</v>
+        <v>103</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>217</v>
+        <v>169</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A76" s="1" t="s">
-        <v>135</v>
+      <c r="A76" s="8" t="s">
+        <v>189</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>140</v>
+        <v>103</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>217</v>
+        <v>169</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A77" s="1" t="s">
-        <v>136</v>
-      </c>
+      <c r="A77" s="8"/>
       <c r="B77" s="1" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>140</v>
+        <v>103</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>217</v>
+        <v>169</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A78" s="1" t="s">
-        <v>137</v>
+      <c r="A78" s="8" t="s">
+        <v>190</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>140</v>
+        <v>103</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>217</v>
+        <v>169</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A79" s="1" t="s">
-        <v>138</v>
-      </c>
+      <c r="A79" s="8"/>
       <c r="B79" s="1" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>140</v>
+        <v>103</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>217</v>
+        <v>169</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A80" s="1" t="s">
-        <v>139</v>
+      <c r="A80" s="8" t="s">
+        <v>191</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>140</v>
+        <v>103</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A81" s="6"/>
-      <c r="B81" s="6"/>
-      <c r="C81" s="6"/>
-      <c r="D81" s="6"/>
-      <c r="E81" s="6"/>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A81" s="8"/>
+      <c r="B81" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="82" spans="1:6" ht="27" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A83" s="8"/>
+      <c r="B83" s="8"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8"/>
+      <c r="E83" s="8"/>
+      <c r="F83" s="8"/>
+    </row>
+    <row r="84" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A84" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A85" s="8"/>
+      <c r="B85" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A86" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A87" s="8"/>
+      <c r="B87" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A88" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A89" s="8"/>
+      <c r="B89" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A90" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A91" s="8"/>
+      <c r="B91" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F91" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A92" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A93" s="8"/>
+      <c r="B93" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F93" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A94" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A95" s="8"/>
+      <c r="B95" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A96" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A97" s="8"/>
+      <c r="B97" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A98" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B99" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F99" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A100" s="8"/>
+      <c r="B100" s="8"/>
+      <c r="C100" s="8"/>
+      <c r="D100" s="8"/>
+      <c r="E100" s="8"/>
+      <c r="F100" s="8"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A101" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A102" s="8"/>
+      <c r="B102" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A103" s="8"/>
+      <c r="B103" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A104" s="8"/>
+      <c r="B104" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E104" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C82" s="1" t="s">
+    </row>
+    <row r="105" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A105" s="8"/>
+      <c r="B105" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A106" s="8"/>
+      <c r="B106" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A107" s="8"/>
+      <c r="B107" s="8"/>
+      <c r="C107" s="8"/>
+      <c r="D107" s="8"/>
+      <c r="E107" s="8"/>
+      <c r="F107" s="8"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A108" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="B108" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A109" s="8"/>
+      <c r="B109" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A110" s="8"/>
+      <c r="B110" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F110" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A111" s="8"/>
+      <c r="B111" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F111" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A112" s="8"/>
+      <c r="B112" s="8"/>
+      <c r="C112" s="8"/>
+      <c r="D112" s="8"/>
+      <c r="E112" s="8"/>
+      <c r="F112" s="8"/>
+    </row>
+    <row r="113" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A113" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E113" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F113" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A114" s="8"/>
+      <c r="B114" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E114" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F114" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A115" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E115" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F115" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A116" s="8"/>
+      <c r="B116" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E116" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F116" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A117" s="8"/>
+      <c r="B117" s="8"/>
+      <c r="C117" s="8"/>
+      <c r="D117" s="8"/>
+      <c r="E117" s="8"/>
+      <c r="F117" s="8"/>
+    </row>
+    <row r="118" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A118" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E118" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A119" s="8"/>
+      <c r="B119" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E119" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A120" s="8"/>
+      <c r="B120" s="8"/>
+      <c r="C120" s="8"/>
+      <c r="D120" s="8"/>
+      <c r="E120" s="8"/>
+      <c r="F120" s="8"/>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A121" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C121" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E82" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="F82" s="5" t="s">
+      <c r="D121" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A122" s="8"/>
+      <c r="B122" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A123" s="8"/>
+      <c r="B123" s="8"/>
+      <c r="C123" s="8"/>
+      <c r="D123" s="8"/>
+      <c r="E123" s="8"/>
+      <c r="F123" s="8"/>
+    </row>
+    <row r="124" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A124" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E124" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A125" s="8"/>
+      <c r="B125" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E125" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A126" s="8"/>
+      <c r="B126" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E126" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A128" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B128" s="1" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A83" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E83" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="F83" s="5" t="s">
+      <c r="C128" s="1" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A84" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E84" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="F84" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A85" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E85" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="F85" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A86" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E86" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="F86" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A87" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E87" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A88" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E88" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A89" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E89" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A90" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E90" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A91" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E91" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="F91" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A92" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E92" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="F92" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A93" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E93" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="F93" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A94" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E94" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="F94" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A95" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E95" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="F95" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A96" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E96" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="F96" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A97" s="6"/>
-      <c r="B97" s="6"/>
-      <c r="C97" s="6"/>
-      <c r="D97" s="6"/>
-      <c r="E97" s="6"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A98" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A99" s="6"/>
-      <c r="B99" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E99" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A100" s="6"/>
-      <c r="B100" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E100" s="4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A101" s="6"/>
-      <c r="B101" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E101" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A102" s="6"/>
-      <c r="B102" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E102" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A103" s="6"/>
-      <c r="B103" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E103" s="4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A104" s="6"/>
-      <c r="B104" s="6"/>
-      <c r="C104" s="6"/>
-      <c r="D104" s="6"/>
-      <c r="E104" s="6"/>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A105" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E105" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F105" s="1" t="s">
+      <c r="E128" s="4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="27" x14ac:dyDescent="0.15">
+      <c r="A129" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E129" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A130" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="B130" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C130" s="1" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A106" s="6"/>
-      <c r="B106" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E106" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F106" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A107" s="6"/>
-      <c r="B107" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E107" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F107" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A108" s="6"/>
-      <c r="B108" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="F108" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A109" s="6"/>
-      <c r="B109" s="6"/>
-      <c r="C109" s="6"/>
-      <c r="D109" s="6"/>
-      <c r="E109" s="6"/>
-    </row>
-    <row r="110" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A110" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E110" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="F110" s="5" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A111" s="6"/>
-      <c r="B111" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E111" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="F111" s="5" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A112" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E112" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="F112" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A113" s="6"/>
-      <c r="B113" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E113" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="F113" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A114" s="6"/>
-      <c r="B114" s="6"/>
-      <c r="C114" s="6"/>
-      <c r="D114" s="6"/>
-      <c r="E114" s="6"/>
-    </row>
-    <row r="115" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A115" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="E115" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A116" s="6"/>
-      <c r="B116" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="E116" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="F116" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A117" s="6"/>
-      <c r="B117" s="6"/>
-      <c r="C117" s="6"/>
-      <c r="D117" s="6"/>
-      <c r="E117" s="6"/>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A118" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="E118" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A119" s="6"/>
-      <c r="B119" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E119" s="2" t="s">
-        <v>208</v>
+      <c r="E130" s="2" t="s">
+        <v>226</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="38">
+    <mergeCell ref="A107:F107"/>
+    <mergeCell ref="A100:F100"/>
+    <mergeCell ref="A83:F83"/>
+    <mergeCell ref="A67:F67"/>
+    <mergeCell ref="A101:A106"/>
+    <mergeCell ref="A108:A111"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="A70:A71"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="A76:A77"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="A80:A81"/>
+    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="A26:A33"/>
+    <mergeCell ref="A34:A41"/>
+    <mergeCell ref="A51:A58"/>
+    <mergeCell ref="A59:A66"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="A50:F50"/>
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="A124:A126"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="A121:A122"/>
+    <mergeCell ref="A113:A114"/>
     <mergeCell ref="A115:A116"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="A109:E109"/>
-    <mergeCell ref="A114:E114"/>
-    <mergeCell ref="A117:E117"/>
-    <mergeCell ref="A110:A111"/>
-    <mergeCell ref="A112:A113"/>
-    <mergeCell ref="A81:E81"/>
-    <mergeCell ref="A97:E97"/>
-    <mergeCell ref="A65:E65"/>
-    <mergeCell ref="A98:A103"/>
-    <mergeCell ref="A105:A108"/>
-    <mergeCell ref="A104:E104"/>
-    <mergeCell ref="A2:A16"/>
-    <mergeCell ref="A18:A32"/>
-    <mergeCell ref="A34:A48"/>
-    <mergeCell ref="A50:A64"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A123:F123"/>
+    <mergeCell ref="A120:F120"/>
+    <mergeCell ref="A117:F117"/>
+    <mergeCell ref="A112:F112"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="F68:F82 F124:F126 F118:F119 F113:F116 F108:F111 F101:F106 F51:F66 F84:F97 F98:F99" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finish basic structure code and update register map.xlsx
</commit_message>
<xml_diff>
--- a/DOC/register map.xlsx
+++ b/DOC/register map.xlsx
@@ -452,10 +452,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>B_VACT _EN_L</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>bit0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -570,10 +566,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>bit3-0</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -816,10 +808,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>A_VACT _EN_L</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>A_FAULT_LED</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -846,6 +834,17 @@
   <si>
     <t>Sideplane_REV_ID0</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A_VACT_EN_L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B_VACT_EN_L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -898,7 +897,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -913,6 +912,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1208,8 +1210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="E122" sqref="E122"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="C121" sqref="C121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1244,14 +1246,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>81</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>20</v>
@@ -1261,7 +1263,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="8"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="1" t="s">
         <v>74</v>
       </c>
@@ -1276,7 +1278,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="8"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="1" t="s">
         <v>75</v>
       </c>
@@ -1291,7 +1293,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="8"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="1" t="s">
         <v>76</v>
       </c>
@@ -1306,7 +1308,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="8"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="1" t="s">
         <v>77</v>
       </c>
@@ -1321,7 +1323,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="8"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="1" t="s">
         <v>78</v>
       </c>
@@ -1336,7 +1338,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" s="8"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="1" t="s">
         <v>79</v>
       </c>
@@ -1351,7 +1353,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9" s="8"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="1" t="s">
         <v>80</v>
       </c>
@@ -1366,8 +1368,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="8" t="s">
-        <v>165</v>
+      <c r="A10" s="9" t="s">
+        <v>163</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>73</v>
@@ -1383,7 +1385,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="8"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="7" t="s">
         <v>74</v>
       </c>
@@ -1398,7 +1400,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="8"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="7" t="s">
         <v>75</v>
       </c>
@@ -1413,7 +1415,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="8"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="7" t="s">
         <v>76</v>
       </c>
@@ -1428,7 +1430,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="8"/>
+      <c r="A14" s="9"/>
       <c r="B14" s="7" t="s">
         <v>77</v>
       </c>
@@ -1443,7 +1445,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="8"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="7" t="s">
         <v>78</v>
       </c>
@@ -1458,7 +1460,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="8"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="7" t="s">
         <v>79</v>
       </c>
@@ -1473,20 +1475,20 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="8"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>198</v>
-      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="8" t="s">
-        <v>166</v>
+      <c r="A18" s="9" t="s">
+        <v>164</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>73</v>
@@ -1502,7 +1504,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="8"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="1" t="s">
         <v>74</v>
       </c>
@@ -1517,7 +1519,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="8"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="1" t="s">
         <v>75</v>
       </c>
@@ -1532,7 +1534,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="8"/>
+      <c r="A21" s="9"/>
       <c r="B21" s="1" t="s">
         <v>76</v>
       </c>
@@ -1547,7 +1549,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="8"/>
+      <c r="A22" s="9"/>
       <c r="B22" s="1" t="s">
         <v>77</v>
       </c>
@@ -1562,7 +1564,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="8"/>
+      <c r="A23" s="9"/>
       <c r="B23" s="1" t="s">
         <v>78</v>
       </c>
@@ -1577,7 +1579,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="8"/>
+      <c r="A24" s="9"/>
       <c r="B24" s="1" t="s">
         <v>79</v>
       </c>
@@ -1592,7 +1594,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="8"/>
+      <c r="A25" s="9"/>
       <c r="B25" s="1" t="s">
         <v>80</v>
       </c>
@@ -1607,8 +1609,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="8" t="s">
-        <v>167</v>
+      <c r="A26" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>73</v>
@@ -1624,7 +1626,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="8"/>
+      <c r="A27" s="9"/>
       <c r="B27" s="7" t="s">
         <v>74</v>
       </c>
@@ -1639,7 +1641,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="8"/>
+      <c r="A28" s="9"/>
       <c r="B28" s="7" t="s">
         <v>75</v>
       </c>
@@ -1654,7 +1656,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="8"/>
+      <c r="A29" s="9"/>
       <c r="B29" s="7" t="s">
         <v>76</v>
       </c>
@@ -1669,7 +1671,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="8"/>
+      <c r="A30" s="9"/>
       <c r="B30" s="7" t="s">
         <v>77</v>
       </c>
@@ -1684,7 +1686,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="8"/>
+      <c r="A31" s="9"/>
       <c r="B31" s="7" t="s">
         <v>78</v>
       </c>
@@ -1699,7 +1701,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="8"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="7" t="s">
         <v>79</v>
       </c>
@@ -1714,20 +1716,20 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="8"/>
+      <c r="A33" s="9"/>
       <c r="B33" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" s="8" t="s">
-        <v>169</v>
+      <c r="A34" s="9" t="s">
+        <v>167</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>73</v>
@@ -1743,7 +1745,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" s="8"/>
+      <c r="A35" s="9"/>
       <c r="B35" s="1" t="s">
         <v>74</v>
       </c>
@@ -1758,7 +1760,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="8"/>
+      <c r="A36" s="9"/>
       <c r="B36" s="1" t="s">
         <v>75</v>
       </c>
@@ -1773,7 +1775,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="8"/>
+      <c r="A37" s="9"/>
       <c r="B37" s="1" t="s">
         <v>76</v>
       </c>
@@ -1788,7 +1790,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="8"/>
+      <c r="A38" s="9"/>
       <c r="B38" s="1" t="s">
         <v>77</v>
       </c>
@@ -1803,7 +1805,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" s="8"/>
+      <c r="A39" s="9"/>
       <c r="B39" s="1" t="s">
         <v>78</v>
       </c>
@@ -1818,7 +1820,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" s="8"/>
+      <c r="A40" s="9"/>
       <c r="B40" s="1" t="s">
         <v>79</v>
       </c>
@@ -1833,7 +1835,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="8"/>
+      <c r="A41" s="9"/>
       <c r="B41" s="1" t="s">
         <v>80</v>
       </c>
@@ -1848,8 +1850,8 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="8" t="s">
-        <v>168</v>
+      <c r="A42" s="9" t="s">
+        <v>166</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>73</v>
@@ -1865,7 +1867,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="8"/>
+      <c r="A43" s="9"/>
       <c r="B43" s="7" t="s">
         <v>74</v>
       </c>
@@ -1880,7 +1882,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="8"/>
+      <c r="A44" s="9"/>
       <c r="B44" s="7" t="s">
         <v>75</v>
       </c>
@@ -1895,7 +1897,7 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="8"/>
+      <c r="A45" s="9"/>
       <c r="B45" s="7" t="s">
         <v>76</v>
       </c>
@@ -1910,7 +1912,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="8"/>
+      <c r="A46" s="9"/>
       <c r="B46" s="7" t="s">
         <v>77</v>
       </c>
@@ -1925,7 +1927,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" s="8"/>
+      <c r="A47" s="9"/>
       <c r="B47" s="7" t="s">
         <v>78</v>
       </c>
@@ -1940,9 +1942,9 @@
       </c>
     </row>
     <row r="48" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="8"/>
+      <c r="A48" s="9"/>
       <c r="B48" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>53</v>
@@ -1955,35 +1957,35 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A49" s="8"/>
+      <c r="A49" s="9"/>
       <c r="B49" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A50" s="8"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8"/>
+      <c r="A50" s="9"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="9" t="s">
         <v>82</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>70</v>
@@ -1992,11 +1994,11 @@
         <v>71</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A52" s="8"/>
+      <c r="A52" s="9"/>
       <c r="B52" s="1" t="s">
         <v>74</v>
       </c>
@@ -2007,14 +2009,14 @@
         <v>70</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A53" s="8"/>
+      <c r="A53" s="9"/>
       <c r="B53" s="1" t="s">
         <v>75</v>
       </c>
@@ -2025,14 +2027,14 @@
         <v>70</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A54" s="8"/>
+      <c r="A54" s="9"/>
       <c r="B54" s="1" t="s">
         <v>76</v>
       </c>
@@ -2043,14 +2045,14 @@
         <v>70</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A55" s="8"/>
+      <c r="A55" s="9"/>
       <c r="B55" s="1" t="s">
         <v>77</v>
       </c>
@@ -2061,14 +2063,14 @@
         <v>70</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A56" s="8"/>
+      <c r="A56" s="9"/>
       <c r="B56" s="1" t="s">
         <v>78</v>
       </c>
@@ -2079,14 +2081,14 @@
         <v>70</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A57" s="8"/>
+      <c r="A57" s="9"/>
       <c r="B57" s="1" t="s">
         <v>79</v>
       </c>
@@ -2097,14 +2099,14 @@
         <v>70</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A58" s="8"/>
+      <c r="A58" s="9"/>
       <c r="B58" s="1" t="s">
         <v>80</v>
       </c>
@@ -2115,15 +2117,15 @@
         <v>70</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A59" s="8" t="s">
-        <v>162</v>
+      <c r="A59" s="9" t="s">
+        <v>160</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>73</v>
@@ -2135,14 +2137,14 @@
         <v>70</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A60" s="8"/>
+      <c r="A60" s="9"/>
       <c r="B60" s="7" t="s">
         <v>74</v>
       </c>
@@ -2153,14 +2155,14 @@
         <v>70</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A61" s="8"/>
+      <c r="A61" s="9"/>
       <c r="B61" s="7" t="s">
         <v>75</v>
       </c>
@@ -2171,14 +2173,14 @@
         <v>70</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A62" s="8"/>
+      <c r="A62" s="9"/>
       <c r="B62" s="7" t="s">
         <v>76</v>
       </c>
@@ -2189,14 +2191,14 @@
         <v>70</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A63" s="8"/>
+      <c r="A63" s="9"/>
       <c r="B63" s="7" t="s">
         <v>77</v>
       </c>
@@ -2207,14 +2209,14 @@
         <v>70</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A64" s="8"/>
+      <c r="A64" s="9"/>
       <c r="B64" s="7" t="s">
         <v>78</v>
       </c>
@@ -2225,16 +2227,16 @@
         <v>70</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="65" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="8"/>
+      <c r="A65" s="9"/>
       <c r="B65" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>69</v>
@@ -2243,45 +2245,45 @@
         <v>70</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A66" s="8"/>
+      <c r="A66" s="9"/>
       <c r="B66" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D66" s="7"/>
       <c r="E66" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A67" s="8"/>
-      <c r="B67" s="8"/>
-      <c r="C67" s="8"/>
-      <c r="D67" s="8"/>
-      <c r="E67" s="8"/>
-      <c r="F67" s="8"/>
+      <c r="A67" s="9"/>
+      <c r="B67" s="9"/>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
     </row>
     <row r="68" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A68" s="8" t="s">
+      <c r="A68" s="9" t="s">
         <v>98</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>96</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>70</v>
@@ -2290,11 +2292,11 @@
         <v>99</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A69" s="8"/>
+      <c r="A69" s="9"/>
       <c r="B69" s="1" t="s">
         <v>97</v>
       </c>
@@ -2308,12 +2310,12 @@
         <v>99</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A70" s="8" t="s">
-        <v>170</v>
+      <c r="A70" s="9" t="s">
+        <v>168</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>96</v>
@@ -2328,11 +2330,11 @@
         <v>99</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A71" s="8"/>
+      <c r="A71" s="9"/>
       <c r="B71" s="1" t="s">
         <v>97</v>
       </c>
@@ -2346,12 +2348,12 @@
         <v>99</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A72" s="8" t="s">
-        <v>171</v>
+      <c r="A72" s="9" t="s">
+        <v>169</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>96</v>
@@ -2366,11 +2368,11 @@
         <v>99</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A73" s="8"/>
+      <c r="A73" s="9"/>
       <c r="B73" s="1" t="s">
         <v>97</v>
       </c>
@@ -2384,12 +2386,12 @@
         <v>99</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A74" s="8" t="s">
-        <v>172</v>
+      <c r="A74" s="9" t="s">
+        <v>170</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>96</v>
@@ -2404,11 +2406,11 @@
         <v>99</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A75" s="8"/>
+      <c r="A75" s="9"/>
       <c r="B75" s="1" t="s">
         <v>97</v>
       </c>
@@ -2422,12 +2424,12 @@
         <v>99</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A76" s="8" t="s">
-        <v>173</v>
+      <c r="A76" s="9" t="s">
+        <v>171</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>96</v>
@@ -2442,11 +2444,11 @@
         <v>99</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A77" s="8"/>
+      <c r="A77" s="9"/>
       <c r="B77" s="1" t="s">
         <v>97</v>
       </c>
@@ -2460,12 +2462,12 @@
         <v>99</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A78" s="8" t="s">
-        <v>174</v>
+      <c r="A78" s="9" t="s">
+        <v>172</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>96</v>
@@ -2480,11 +2482,11 @@
         <v>99</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A79" s="8"/>
+      <c r="A79" s="9"/>
       <c r="B79" s="1" t="s">
         <v>97</v>
       </c>
@@ -2498,12 +2500,12 @@
         <v>99</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A80" s="8" t="s">
-        <v>175</v>
+      <c r="A80" s="9" t="s">
+        <v>173</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>96</v>
@@ -2518,11 +2520,11 @@
         <v>99</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A81" s="8"/>
+      <c r="A81" s="9"/>
       <c r="B81" s="1" t="s">
         <v>97</v>
       </c>
@@ -2536,18 +2538,18 @@
         <v>99</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="27" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>96</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>70</v>
@@ -2556,26 +2558,26 @@
         <v>99</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A83" s="8"/>
-      <c r="B83" s="8"/>
-      <c r="C83" s="8"/>
-      <c r="D83" s="8"/>
-      <c r="E83" s="8"/>
-      <c r="F83" s="8"/>
+      <c r="A83" s="9"/>
+      <c r="B83" s="9"/>
+      <c r="C83" s="9"/>
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="9"/>
     </row>
     <row r="84" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A84" s="8" t="s">
+      <c r="A84" s="9" t="s">
         <v>100</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>96</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>115</v>
@@ -2584,11 +2586,11 @@
         <v>121</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A85" s="8"/>
+      <c r="A85" s="9"/>
       <c r="B85" s="1" t="s">
         <v>97</v>
       </c>
@@ -2602,12 +2604,12 @@
         <v>121</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A86" s="8" t="s">
-        <v>177</v>
+      <c r="A86" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>96</v>
@@ -2622,11 +2624,11 @@
         <v>121</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A87" s="8"/>
+      <c r="A87" s="9"/>
       <c r="B87" s="1" t="s">
         <v>97</v>
       </c>
@@ -2640,11 +2642,11 @@
         <v>121</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A88" s="8" t="s">
+      <c r="A88" s="9" t="s">
         <v>116</v>
       </c>
       <c r="B88" s="1" t="s">
@@ -2660,11 +2662,11 @@
         <v>121</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A89" s="8"/>
+      <c r="A89" s="9"/>
       <c r="B89" s="1" t="s">
         <v>97</v>
       </c>
@@ -2678,11 +2680,11 @@
         <v>121</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A90" s="8" t="s">
+      <c r="A90" s="9" t="s">
         <v>117</v>
       </c>
       <c r="B90" s="1" t="s">
@@ -2698,11 +2700,11 @@
         <v>121</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A91" s="8"/>
+      <c r="A91" s="9"/>
       <c r="B91" s="1" t="s">
         <v>97</v>
       </c>
@@ -2716,11 +2718,11 @@
         <v>121</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A92" s="8" t="s">
+      <c r="A92" s="9" t="s">
         <v>118</v>
       </c>
       <c r="B92" s="1" t="s">
@@ -2736,11 +2738,11 @@
         <v>121</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A93" s="8"/>
+      <c r="A93" s="9"/>
       <c r="B93" s="1" t="s">
         <v>97</v>
       </c>
@@ -2754,11 +2756,11 @@
         <v>121</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A94" s="8" t="s">
+      <c r="A94" s="9" t="s">
         <v>119</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -2774,11 +2776,11 @@
         <v>121</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A95" s="8"/>
+      <c r="A95" s="9"/>
       <c r="B95" s="1" t="s">
         <v>97</v>
       </c>
@@ -2792,11 +2794,11 @@
         <v>121</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A96" s="8" t="s">
+      <c r="A96" s="9" t="s">
         <v>120</v>
       </c>
       <c r="B96" s="1" t="s">
@@ -2812,11 +2814,11 @@
         <v>121</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A97" s="8"/>
+      <c r="A97" s="9"/>
       <c r="B97" s="1" t="s">
         <v>97</v>
       </c>
@@ -2830,12 +2832,12 @@
         <v>121</v>
       </c>
       <c r="F97" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="98" spans="1:6" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.15">
       <c r="A98" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>96</v>
@@ -2850,7 +2852,7 @@
         <v>121</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.15">
@@ -2858,57 +2860,57 @@
         <v>97</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A100" s="8"/>
-      <c r="B100" s="8"/>
-      <c r="C100" s="8"/>
-      <c r="D100" s="8"/>
-      <c r="E100" s="8"/>
-      <c r="F100" s="8"/>
+      <c r="A100" s="9"/>
+      <c r="B100" s="9"/>
+      <c r="C100" s="9"/>
+      <c r="D100" s="9"/>
+      <c r="E100" s="9"/>
+      <c r="F100" s="9"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A101" s="8" t="s">
+      <c r="A101" s="9" t="s">
         <v>124</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>125</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>123</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A102" s="8"/>
+      <c r="A102" s="9"/>
       <c r="B102" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>123</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A103" s="8"/>
+      <c r="A103" s="9"/>
       <c r="B103" s="1" t="s">
         <v>75</v>
       </c>
@@ -2919,11 +2921,11 @@
         <v>123</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A104" s="8"/>
+      <c r="A104" s="9"/>
       <c r="B104" s="1" t="s">
         <v>76</v>
       </c>
@@ -2934,11 +2936,11 @@
         <v>123</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A105" s="8"/>
+      <c r="A105" s="9"/>
       <c r="B105" s="1" t="s">
         <v>77</v>
       </c>
@@ -2949,11 +2951,11 @@
         <v>123</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A106" s="8"/>
+      <c r="A106" s="9"/>
       <c r="B106" s="1" t="s">
         <v>78</v>
       </c>
@@ -2964,57 +2966,57 @@
         <v>123</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A107" s="8"/>
-      <c r="B107" s="8"/>
-      <c r="C107" s="8"/>
-      <c r="D107" s="8"/>
-      <c r="E107" s="8"/>
-      <c r="F107" s="8"/>
+      <c r="A107" s="9"/>
+      <c r="B107" s="9"/>
+      <c r="C107" s="9"/>
+      <c r="D107" s="9"/>
+      <c r="E107" s="9"/>
+      <c r="F107" s="9"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A108" s="8" t="s">
-        <v>132</v>
+      <c r="A108" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>115</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>159</v>
+        <v>182</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A109" s="8"/>
+      <c r="A109" s="9"/>
       <c r="B109" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>115</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A110" s="8"/>
+      <c r="A110" s="9"/>
       <c r="B110" s="1" t="s">
         <v>75</v>
       </c>
@@ -3025,318 +3027,300 @@
         <v>115</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F110" s="5" t="s">
-        <v>152</v>
+        <v>133</v>
+      </c>
+      <c r="F110" s="8" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A111" s="8"/>
+      <c r="A111" s="9"/>
       <c r="B111" s="1" t="s">
         <v>76</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>130</v>
+        <v>225</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>115</v>
       </c>
       <c r="E111" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F111" s="8" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A112" s="9"/>
+      <c r="B112" s="9"/>
+      <c r="C112" s="9"/>
+      <c r="D112" s="9"/>
+      <c r="E112" s="9"/>
+      <c r="F112" s="9"/>
+    </row>
+    <row r="113" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A113" s="9" t="s">
         <v>136</v>
-      </c>
-      <c r="F111" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A112" s="8"/>
-      <c r="B112" s="8"/>
-      <c r="C112" s="8"/>
-      <c r="D112" s="8"/>
-      <c r="E112" s="8"/>
-      <c r="F112" s="8"/>
-    </row>
-    <row r="113" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A113" s="8" t="s">
-        <v>137</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>96</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E113" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F113" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A114" s="8"/>
+      <c r="A114" s="9"/>
       <c r="B114" s="1" t="s">
         <v>97</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E114" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F114" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A115" s="8" t="s">
-        <v>138</v>
+      <c r="A115" s="9" t="s">
+        <v>137</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>96</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E115" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A116" s="8"/>
+      <c r="A116" s="9"/>
       <c r="B116" s="1" t="s">
         <v>97</v>
       </c>
       <c r="C116" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D116" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D116" s="1" t="s">
+      <c r="E116" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F116" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A117" s="9"/>
+      <c r="B117" s="9"/>
+      <c r="C117" s="9"/>
+      <c r="D117" s="9"/>
+      <c r="E117" s="9"/>
+      <c r="F117" s="9"/>
+    </row>
+    <row r="118" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A118" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D118" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E116" s="4" t="s">
+      <c r="E118" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="F116" s="5" t="s">
+      <c r="F118" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A117" s="8"/>
-      <c r="B117" s="8"/>
-      <c r="C117" s="8"/>
-      <c r="D117" s="8"/>
-      <c r="E117" s="8"/>
-      <c r="F117" s="8"/>
-    </row>
-    <row r="118" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A118" s="8" t="s">
+    <row r="119" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A119" s="9"/>
+      <c r="B119" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E119" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A120" s="9"/>
+      <c r="B120" s="9"/>
+      <c r="C120" s="9"/>
+      <c r="D120" s="9"/>
+      <c r="E120" s="9"/>
+      <c r="F120" s="9"/>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A121" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="B118" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E118" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="F118" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A119" s="8"/>
-      <c r="B119" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E119" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A120" s="8"/>
-      <c r="B120" s="8"/>
-      <c r="C120" s="8"/>
-      <c r="D120" s="8"/>
-      <c r="E120" s="8"/>
-      <c r="F120" s="8"/>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A121" s="8" t="s">
+      <c r="B121" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="C121" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E121" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C121" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E121" s="2" t="s">
-        <v>145</v>
-      </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A122" s="8"/>
+      <c r="A122" s="9"/>
       <c r="B122" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A123" s="8"/>
-      <c r="B123" s="8"/>
-      <c r="C123" s="8"/>
-      <c r="D123" s="8"/>
-      <c r="E123" s="8"/>
-      <c r="F123" s="8"/>
+      <c r="A123" s="9"/>
+      <c r="B123" s="9"/>
+      <c r="C123" s="9"/>
+      <c r="D123" s="9"/>
+      <c r="E123" s="9"/>
+      <c r="F123" s="9"/>
     </row>
     <row r="124" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A124" s="8" t="s">
+      <c r="A124" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C124" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B124" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>181</v>
-      </c>
       <c r="E124" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A125" s="8"/>
+      <c r="A125" s="9"/>
       <c r="B125" s="6" t="s">
         <v>74</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E125" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A126" s="8"/>
+      <c r="A126" s="9"/>
       <c r="B126" s="6" t="s">
         <v>75</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E126" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="128" spans="1:6" ht="27" x14ac:dyDescent="0.15">
       <c r="A128" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E128" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="27" x14ac:dyDescent="0.15">
       <c r="A129" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C129" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B129" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="C129" s="1" t="s">
+      <c r="E129" s="4" t="s">
         <v>206</v>
-      </c>
-      <c r="E129" s="4" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A130" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B130" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C130" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B130" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="E130" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="A112:F112"/>
-    <mergeCell ref="A124:A126"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="A121:A122"/>
-    <mergeCell ref="A113:A114"/>
-    <mergeCell ref="A115:A116"/>
-    <mergeCell ref="A123:F123"/>
-    <mergeCell ref="A120:F120"/>
-    <mergeCell ref="A117:F117"/>
-    <mergeCell ref="A51:A58"/>
-    <mergeCell ref="A59:A66"/>
-    <mergeCell ref="A42:A49"/>
-    <mergeCell ref="A50:F50"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A10:A17"/>
-    <mergeCell ref="A18:A25"/>
-    <mergeCell ref="A26:A33"/>
-    <mergeCell ref="A34:A41"/>
+    <mergeCell ref="A101:A106"/>
     <mergeCell ref="A108:A111"/>
     <mergeCell ref="A68:A69"/>
     <mergeCell ref="A70:A71"/>
@@ -3353,15 +3337,33 @@
     <mergeCell ref="A96:A97"/>
     <mergeCell ref="A107:F107"/>
     <mergeCell ref="A100:F100"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="A26:A33"/>
+    <mergeCell ref="A34:A41"/>
+    <mergeCell ref="A51:A58"/>
+    <mergeCell ref="A59:A66"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="A50:F50"/>
+    <mergeCell ref="A90:A91"/>
     <mergeCell ref="A83:F83"/>
     <mergeCell ref="A67:F67"/>
-    <mergeCell ref="A101:A106"/>
+    <mergeCell ref="A112:F112"/>
+    <mergeCell ref="A124:A126"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="A121:A122"/>
+    <mergeCell ref="A113:A114"/>
+    <mergeCell ref="A115:A116"/>
+    <mergeCell ref="A123:F123"/>
+    <mergeCell ref="A120:F120"/>
+    <mergeCell ref="A117:F117"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="F68:F82 F124:F126 F118:F119 F113:F116 F108:F111 F101:F106 F51:F66 F84:F97 F98:F99" numberStoredAsText="1"/>
+    <ignoredError sqref="F68:F82 F124:F126 F118:F119 F113:F116 F101:F106 F51:F66 F84:F97 F98:F99" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update spec to v0.3, add section 5.5 for enclosure led toggle rate
</commit_message>
<xml_diff>
--- a/DOC/register map.xlsx
+++ b/DOC/register map.xlsx
@@ -534,12 +534,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>L: Normal System Operation 
-PWM: Sled Identify
-H: Reserved</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -670,12 +664,6 @@
   </si>
   <si>
     <t>0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>L: Reserved
-PWM: Reserved
-H: Any failure in whole enclosure</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -844,6 +832,18 @@
   </si>
   <si>
     <t>ENCLOSURE_FAULT_LED</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>L: Reserved
+PWM: 0.9sec ON, 0.1sec OFF, Loop
+H: Any failure in whole enclosure</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>L: Normal System Operation 
+PWM: 0.9sec ON, 0.1sec OFF, Loop
+H: Reserved</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1211,7 +1211,7 @@
   <dimension ref="A1:F130"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="C119" sqref="C119"/>
+      <selection activeCell="G118" sqref="G118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1253,7 +1253,7 @@
         <v>73</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>20</v>
@@ -1369,7 +1369,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>73</v>
@@ -1477,18 +1477,18 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" s="9"/>
       <c r="B17" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>73</v>
@@ -1610,7 +1610,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>73</v>
@@ -1718,18 +1718,18 @@
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" s="9"/>
       <c r="B33" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>73</v>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A42" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>73</v>
@@ -1944,7 +1944,7 @@
     <row r="48" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A48" s="9"/>
       <c r="B48" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>53</v>
@@ -1959,14 +1959,14 @@
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A49" s="9"/>
       <c r="B49" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
@@ -1985,7 +1985,7 @@
         <v>73</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>70</v>
@@ -1994,7 +1994,7 @@
         <v>71</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
@@ -2009,10 +2009,10 @@
         <v>70</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
@@ -2027,10 +2027,10 @@
         <v>70</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
@@ -2045,10 +2045,10 @@
         <v>70</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
@@ -2063,10 +2063,10 @@
         <v>70</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
@@ -2081,10 +2081,10 @@
         <v>70</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
@@ -2099,10 +2099,10 @@
         <v>70</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
@@ -2117,15 +2117,15 @@
         <v>70</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A59" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>73</v>
@@ -2137,10 +2137,10 @@
         <v>70</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
@@ -2155,10 +2155,10 @@
         <v>70</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
@@ -2173,10 +2173,10 @@
         <v>70</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
@@ -2191,10 +2191,10 @@
         <v>70</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.15">
@@ -2209,10 +2209,10 @@
         <v>70</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.15">
@@ -2227,16 +2227,16 @@
         <v>70</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="65" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A65" s="9"/>
       <c r="B65" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>69</v>
@@ -2245,26 +2245,26 @@
         <v>70</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A66" s="9"/>
       <c r="B66" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D66" s="7"/>
       <c r="E66" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.15">
@@ -2283,7 +2283,7 @@
         <v>96</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>70</v>
@@ -2292,7 +2292,7 @@
         <v>99</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -2310,12 +2310,12 @@
         <v>99</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="27" x14ac:dyDescent="0.15">
       <c r="A70" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>96</v>
@@ -2330,7 +2330,7 @@
         <v>99</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -2348,12 +2348,12 @@
         <v>99</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="27" x14ac:dyDescent="0.15">
       <c r="A72" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>96</v>
@@ -2368,7 +2368,7 @@
         <v>99</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -2386,12 +2386,12 @@
         <v>99</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="27" x14ac:dyDescent="0.15">
       <c r="A74" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>96</v>
@@ -2406,7 +2406,7 @@
         <v>99</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -2424,12 +2424,12 @@
         <v>99</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="27" x14ac:dyDescent="0.15">
       <c r="A76" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>96</v>
@@ -2444,7 +2444,7 @@
         <v>99</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -2462,12 +2462,12 @@
         <v>99</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="27" x14ac:dyDescent="0.15">
       <c r="A78" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>96</v>
@@ -2482,7 +2482,7 @@
         <v>99</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -2500,12 +2500,12 @@
         <v>99</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="27" x14ac:dyDescent="0.15">
       <c r="A80" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>96</v>
@@ -2520,7 +2520,7 @@
         <v>99</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -2538,18 +2538,18 @@
         <v>99</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="27" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>96</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>70</v>
@@ -2558,7 +2558,7 @@
         <v>99</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.15">
@@ -2577,7 +2577,7 @@
         <v>96</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>115</v>
@@ -2586,7 +2586,7 @@
         <v>121</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -2604,12 +2604,12 @@
         <v>121</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="27" x14ac:dyDescent="0.15">
       <c r="A86" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>96</v>
@@ -2624,7 +2624,7 @@
         <v>121</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -2642,7 +2642,7 @@
         <v>121</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -2662,7 +2662,7 @@
         <v>121</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -2680,7 +2680,7 @@
         <v>121</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -2700,7 +2700,7 @@
         <v>121</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -2718,7 +2718,7 @@
         <v>121</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -2738,7 +2738,7 @@
         <v>121</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -2756,7 +2756,7 @@
         <v>121</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -2776,7 +2776,7 @@
         <v>121</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -2794,7 +2794,7 @@
         <v>121</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -2814,7 +2814,7 @@
         <v>121</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -2832,12 +2832,12 @@
         <v>121</v>
       </c>
       <c r="F97" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="98" spans="1:6" s="7" customFormat="1" ht="27" x14ac:dyDescent="0.15">
       <c r="A98" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>96</v>
@@ -2852,7 +2852,7 @@
         <v>121</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.15">
@@ -2860,13 +2860,13 @@
         <v>97</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.15">
@@ -2885,13 +2885,13 @@
         <v>125</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>123</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -2900,13 +2900,13 @@
         <v>74</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>123</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -2951,7 +2951,7 @@
         <v>123</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -2985,7 +2985,7 @@
         <v>130</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>115</v>
@@ -2994,7 +2994,7 @@
         <v>133</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.15">
@@ -3003,7 +3003,7 @@
         <v>74</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>115</v>
@@ -3012,7 +3012,7 @@
         <v>134</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.15">
@@ -3030,7 +3030,7 @@
         <v>133</v>
       </c>
       <c r="F110" s="8" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.15">
@@ -3039,7 +3039,7 @@
         <v>76</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>115</v>
@@ -3048,7 +3048,7 @@
         <v>135</v>
       </c>
       <c r="F111" s="8" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.15">
@@ -3067,7 +3067,7 @@
         <v>96</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>139</v>
@@ -3076,7 +3076,7 @@
         <v>148</v>
       </c>
       <c r="F113" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -3085,7 +3085,7 @@
         <v>97</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>139</v>
@@ -3094,7 +3094,7 @@
         <v>149</v>
       </c>
       <c r="F114" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -3105,7 +3105,7 @@
         <v>96</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>139</v>
@@ -3114,7 +3114,7 @@
         <v>148</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -3132,7 +3132,7 @@
         <v>149</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.15">
@@ -3148,37 +3148,37 @@
         <v>141</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>140</v>
       </c>
       <c r="E118" s="4" t="s">
-        <v>150</v>
+        <v>226</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A119" s="9"/>
       <c r="B119" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>140</v>
       </c>
       <c r="E119" s="4" t="s">
-        <v>185</v>
+        <v>225</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.15">
@@ -3197,7 +3197,7 @@
         <v>143</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>145</v>
@@ -3212,7 +3212,7 @@
         <v>74</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>146</v>
@@ -3231,19 +3231,19 @@
     </row>
     <row r="124" spans="1:6" ht="27" x14ac:dyDescent="0.15">
       <c r="A124" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B124" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="C124" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="C124" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="E124" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -3252,13 +3252,13 @@
         <v>74</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E125" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -3267,81 +3267,59 @@
         <v>75</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E126" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="128" spans="1:6" ht="27" x14ac:dyDescent="0.15">
       <c r="A128" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E128" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="27" x14ac:dyDescent="0.15">
       <c r="A129" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C129" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B129" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="C129" s="1" t="s">
+      <c r="E129" s="4" t="s">
         <v>204</v>
-      </c>
-      <c r="E129" s="4" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A130" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B130" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C130" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B130" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>205</v>
-      </c>
       <c r="E130" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="A112:F112"/>
-    <mergeCell ref="A124:A126"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="A121:A122"/>
-    <mergeCell ref="A113:A114"/>
-    <mergeCell ref="A115:A116"/>
-    <mergeCell ref="A123:F123"/>
-    <mergeCell ref="A120:F120"/>
-    <mergeCell ref="A117:F117"/>
-    <mergeCell ref="A100:F100"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A10:A17"/>
-    <mergeCell ref="A18:A25"/>
-    <mergeCell ref="A26:A33"/>
-    <mergeCell ref="A34:A41"/>
-    <mergeCell ref="A51:A58"/>
-    <mergeCell ref="A59:A66"/>
-    <mergeCell ref="A42:A49"/>
-    <mergeCell ref="A50:F50"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="A83:F83"/>
-    <mergeCell ref="A67:F67"/>
     <mergeCell ref="A101:A106"/>
     <mergeCell ref="A108:A111"/>
     <mergeCell ref="A68:A69"/>
@@ -3358,6 +3336,28 @@
     <mergeCell ref="A94:A95"/>
     <mergeCell ref="A96:A97"/>
     <mergeCell ref="A107:F107"/>
+    <mergeCell ref="A100:F100"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="A26:A33"/>
+    <mergeCell ref="A34:A41"/>
+    <mergeCell ref="A51:A58"/>
+    <mergeCell ref="A59:A66"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="A50:F50"/>
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="A83:F83"/>
+    <mergeCell ref="A67:F67"/>
+    <mergeCell ref="A112:F112"/>
+    <mergeCell ref="A124:A126"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="A121:A122"/>
+    <mergeCell ref="A113:A114"/>
+    <mergeCell ref="A115:A116"/>
+    <mergeCell ref="A123:F123"/>
+    <mergeCell ref="A120:F120"/>
+    <mergeCell ref="A117:F117"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
V0.4 spec and image release Add software reset register
</commit_message>
<xml_diff>
--- a/DOC/register map.xlsx
+++ b/DOC/register map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="233">
   <si>
     <t>Offset</t>
   </si>
@@ -844,6 +844,30 @@
     <t>L: Normal System Operation 
 PWM: 0.9sec ON, 0.1sec OFF, Loop
 H: Reserved</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bit0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Software_reset</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>If write '1', all registers will be set to default value</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -897,7 +921,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -926,6 +950,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1208,10 +1241,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F130"/>
+  <dimension ref="A1:F132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="G118" sqref="G118"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection sqref="A1:F132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1246,7 +1279,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>81</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1263,7 +1296,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="9"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="1" t="s">
         <v>74</v>
       </c>
@@ -1278,7 +1311,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="9"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="1" t="s">
         <v>75</v>
       </c>
@@ -1293,7 +1326,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="9"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="1" t="s">
         <v>76</v>
       </c>
@@ -1308,7 +1341,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="9"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="1" t="s">
         <v>77</v>
       </c>
@@ -1323,7 +1356,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="9"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="1" t="s">
         <v>78</v>
       </c>
@@ -1338,7 +1371,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" s="9"/>
+      <c r="A8" s="10"/>
       <c r="B8" s="1" t="s">
         <v>79</v>
       </c>
@@ -1353,7 +1386,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9" s="9"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="1" t="s">
         <v>80</v>
       </c>
@@ -1368,7 +1401,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="10" t="s">
         <v>162</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -1385,7 +1418,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="9"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="7" t="s">
         <v>74</v>
       </c>
@@ -1400,7 +1433,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="9"/>
+      <c r="A12" s="10"/>
       <c r="B12" s="7" t="s">
         <v>75</v>
       </c>
@@ -1415,7 +1448,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="9"/>
+      <c r="A13" s="10"/>
       <c r="B13" s="7" t="s">
         <v>76</v>
       </c>
@@ -1430,7 +1463,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="9"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="7" t="s">
         <v>77</v>
       </c>
@@ -1445,7 +1478,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="9"/>
+      <c r="A15" s="10"/>
       <c r="B15" s="7" t="s">
         <v>78</v>
       </c>
@@ -1460,7 +1493,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="9"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="7" t="s">
         <v>79</v>
       </c>
@@ -1475,7 +1508,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="9"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="1" t="s">
         <v>191</v>
       </c>
@@ -1487,7 +1520,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="10" t="s">
         <v>163</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1504,7 +1537,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="9"/>
+      <c r="A19" s="10"/>
       <c r="B19" s="1" t="s">
         <v>74</v>
       </c>
@@ -1519,7 +1552,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="9"/>
+      <c r="A20" s="10"/>
       <c r="B20" s="1" t="s">
         <v>75</v>
       </c>
@@ -1534,7 +1567,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="9"/>
+      <c r="A21" s="10"/>
       <c r="B21" s="1" t="s">
         <v>76</v>
       </c>
@@ -1549,7 +1582,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="9"/>
+      <c r="A22" s="10"/>
       <c r="B22" s="1" t="s">
         <v>77</v>
       </c>
@@ -1564,7 +1597,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="9"/>
+      <c r="A23" s="10"/>
       <c r="B23" s="1" t="s">
         <v>78</v>
       </c>
@@ -1579,7 +1612,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="9"/>
+      <c r="A24" s="10"/>
       <c r="B24" s="1" t="s">
         <v>79</v>
       </c>
@@ -1594,7 +1627,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="9"/>
+      <c r="A25" s="10"/>
       <c r="B25" s="1" t="s">
         <v>80</v>
       </c>
@@ -1609,7 +1642,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="10" t="s">
         <v>164</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -1626,7 +1659,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="9"/>
+      <c r="A27" s="10"/>
       <c r="B27" s="7" t="s">
         <v>74</v>
       </c>
@@ -1641,7 +1674,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="9"/>
+      <c r="A28" s="10"/>
       <c r="B28" s="7" t="s">
         <v>75</v>
       </c>
@@ -1656,7 +1689,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="9"/>
+      <c r="A29" s="10"/>
       <c r="B29" s="7" t="s">
         <v>76</v>
       </c>
@@ -1671,7 +1704,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="9"/>
+      <c r="A30" s="10"/>
       <c r="B30" s="7" t="s">
         <v>77</v>
       </c>
@@ -1686,7 +1719,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="9"/>
+      <c r="A31" s="10"/>
       <c r="B31" s="7" t="s">
         <v>78</v>
       </c>
@@ -1701,7 +1734,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="9"/>
+      <c r="A32" s="10"/>
       <c r="B32" s="7" t="s">
         <v>79</v>
       </c>
@@ -1716,7 +1749,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="9"/>
+      <c r="A33" s="10"/>
       <c r="B33" s="1" t="s">
         <v>193</v>
       </c>
@@ -1728,7 +1761,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="10" t="s">
         <v>166</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1745,7 +1778,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" s="9"/>
+      <c r="A35" s="10"/>
       <c r="B35" s="1" t="s">
         <v>74</v>
       </c>
@@ -1760,7 +1793,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="9"/>
+      <c r="A36" s="10"/>
       <c r="B36" s="1" t="s">
         <v>75</v>
       </c>
@@ -1775,7 +1808,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="9"/>
+      <c r="A37" s="10"/>
       <c r="B37" s="1" t="s">
         <v>76</v>
       </c>
@@ -1790,7 +1823,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="9"/>
+      <c r="A38" s="10"/>
       <c r="B38" s="1" t="s">
         <v>77</v>
       </c>
@@ -1805,7 +1838,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" s="9"/>
+      <c r="A39" s="10"/>
       <c r="B39" s="1" t="s">
         <v>78</v>
       </c>
@@ -1820,7 +1853,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" s="9"/>
+      <c r="A40" s="10"/>
       <c r="B40" s="1" t="s">
         <v>79</v>
       </c>
@@ -1835,7 +1868,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="9"/>
+      <c r="A41" s="10"/>
       <c r="B41" s="1" t="s">
         <v>80</v>
       </c>
@@ -1850,7 +1883,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="10" t="s">
         <v>165</v>
       </c>
       <c r="B42" s="7" t="s">
@@ -1867,7 +1900,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="9"/>
+      <c r="A43" s="10"/>
       <c r="B43" s="7" t="s">
         <v>74</v>
       </c>
@@ -1882,7 +1915,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="9"/>
+      <c r="A44" s="10"/>
       <c r="B44" s="7" t="s">
         <v>75</v>
       </c>
@@ -1897,7 +1930,7 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="9"/>
+      <c r="A45" s="10"/>
       <c r="B45" s="7" t="s">
         <v>76</v>
       </c>
@@ -1912,7 +1945,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="9"/>
+      <c r="A46" s="10"/>
       <c r="B46" s="7" t="s">
         <v>77</v>
       </c>
@@ -1927,7 +1960,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" s="9"/>
+      <c r="A47" s="10"/>
       <c r="B47" s="7" t="s">
         <v>78</v>
       </c>
@@ -1942,7 +1975,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="9"/>
+      <c r="A48" s="10"/>
       <c r="B48" s="7" t="s">
         <v>195</v>
       </c>
@@ -1957,7 +1990,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A49" s="9"/>
+      <c r="A49" s="10"/>
       <c r="B49" s="7" t="s">
         <v>193</v>
       </c>
@@ -1970,15 +2003,15 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A50" s="9"/>
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="10" t="s">
         <v>82</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -1998,7 +2031,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A52" s="9"/>
+      <c r="A52" s="10"/>
       <c r="B52" s="1" t="s">
         <v>74</v>
       </c>
@@ -2016,7 +2049,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A53" s="9"/>
+      <c r="A53" s="10"/>
       <c r="B53" s="1" t="s">
         <v>75</v>
       </c>
@@ -2034,7 +2067,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A54" s="9"/>
+      <c r="A54" s="10"/>
       <c r="B54" s="1" t="s">
         <v>76</v>
       </c>
@@ -2052,7 +2085,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A55" s="9"/>
+      <c r="A55" s="10"/>
       <c r="B55" s="1" t="s">
         <v>77</v>
       </c>
@@ -2070,7 +2103,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A56" s="9"/>
+      <c r="A56" s="10"/>
       <c r="B56" s="1" t="s">
         <v>78</v>
       </c>
@@ -2088,7 +2121,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A57" s="9"/>
+      <c r="A57" s="10"/>
       <c r="B57" s="1" t="s">
         <v>79</v>
       </c>
@@ -2106,7 +2139,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A58" s="9"/>
+      <c r="A58" s="10"/>
       <c r="B58" s="1" t="s">
         <v>80</v>
       </c>
@@ -2124,7 +2157,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A59" s="9" t="s">
+      <c r="A59" s="10" t="s">
         <v>159</v>
       </c>
       <c r="B59" s="7" t="s">
@@ -2144,7 +2177,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A60" s="9"/>
+      <c r="A60" s="10"/>
       <c r="B60" s="7" t="s">
         <v>74</v>
       </c>
@@ -2162,7 +2195,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A61" s="9"/>
+      <c r="A61" s="10"/>
       <c r="B61" s="7" t="s">
         <v>75</v>
       </c>
@@ -2180,7 +2213,7 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A62" s="9"/>
+      <c r="A62" s="10"/>
       <c r="B62" s="7" t="s">
         <v>76</v>
       </c>
@@ -2198,7 +2231,7 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A63" s="9"/>
+      <c r="A63" s="10"/>
       <c r="B63" s="7" t="s">
         <v>77</v>
       </c>
@@ -2216,7 +2249,7 @@
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A64" s="9"/>
+      <c r="A64" s="10"/>
       <c r="B64" s="7" t="s">
         <v>78</v>
       </c>
@@ -2234,7 +2267,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="9"/>
+      <c r="A65" s="10"/>
       <c r="B65" s="7" t="s">
         <v>195</v>
       </c>
@@ -2252,7 +2285,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A66" s="9"/>
+      <c r="A66" s="10"/>
       <c r="B66" s="7" t="s">
         <v>193</v>
       </c>
@@ -2268,15 +2301,15 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A67" s="9"/>
-      <c r="B67" s="9"/>
-      <c r="C67" s="9"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="9"/>
+      <c r="A67" s="10"/>
+      <c r="B67" s="10"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="10"/>
     </row>
     <row r="68" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A68" s="9" t="s">
+      <c r="A68" s="10" t="s">
         <v>98</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -2296,7 +2329,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A69" s="9"/>
+      <c r="A69" s="10"/>
       <c r="B69" s="1" t="s">
         <v>97</v>
       </c>
@@ -2314,7 +2347,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A70" s="9" t="s">
+      <c r="A70" s="10" t="s">
         <v>167</v>
       </c>
       <c r="B70" s="1" t="s">
@@ -2334,7 +2367,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A71" s="9"/>
+      <c r="A71" s="10"/>
       <c r="B71" s="1" t="s">
         <v>97</v>
       </c>
@@ -2352,7 +2385,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A72" s="9" t="s">
+      <c r="A72" s="10" t="s">
         <v>168</v>
       </c>
       <c r="B72" s="1" t="s">
@@ -2372,7 +2405,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A73" s="9"/>
+      <c r="A73" s="10"/>
       <c r="B73" s="1" t="s">
         <v>97</v>
       </c>
@@ -2390,7 +2423,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A74" s="9" t="s">
+      <c r="A74" s="10" t="s">
         <v>169</v>
       </c>
       <c r="B74" s="1" t="s">
@@ -2410,7 +2443,7 @@
       </c>
     </row>
     <row r="75" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A75" s="9"/>
+      <c r="A75" s="10"/>
       <c r="B75" s="1" t="s">
         <v>97</v>
       </c>
@@ -2428,7 +2461,7 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A76" s="9" t="s">
+      <c r="A76" s="10" t="s">
         <v>170</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -2448,7 +2481,7 @@
       </c>
     </row>
     <row r="77" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A77" s="9"/>
+      <c r="A77" s="10"/>
       <c r="B77" s="1" t="s">
         <v>97</v>
       </c>
@@ -2466,7 +2499,7 @@
       </c>
     </row>
     <row r="78" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A78" s="9" t="s">
+      <c r="A78" s="10" t="s">
         <v>171</v>
       </c>
       <c r="B78" s="1" t="s">
@@ -2486,7 +2519,7 @@
       </c>
     </row>
     <row r="79" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A79" s="9"/>
+      <c r="A79" s="10"/>
       <c r="B79" s="1" t="s">
         <v>97</v>
       </c>
@@ -2504,7 +2537,7 @@
       </c>
     </row>
     <row r="80" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A80" s="9" t="s">
+      <c r="A80" s="10" t="s">
         <v>172</v>
       </c>
       <c r="B80" s="1" t="s">
@@ -2524,7 +2557,7 @@
       </c>
     </row>
     <row r="81" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A81" s="9"/>
+      <c r="A81" s="10"/>
       <c r="B81" s="1" t="s">
         <v>97</v>
       </c>
@@ -2562,15 +2595,15 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A83" s="9"/>
-      <c r="B83" s="9"/>
-      <c r="C83" s="9"/>
-      <c r="D83" s="9"/>
-      <c r="E83" s="9"/>
-      <c r="F83" s="9"/>
+      <c r="A83" s="10"/>
+      <c r="B83" s="10"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="10"/>
+      <c r="E83" s="10"/>
+      <c r="F83" s="10"/>
     </row>
     <row r="84" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A84" s="9" t="s">
+      <c r="A84" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B84" s="1" t="s">
@@ -2590,7 +2623,7 @@
       </c>
     </row>
     <row r="85" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A85" s="9"/>
+      <c r="A85" s="10"/>
       <c r="B85" s="1" t="s">
         <v>97</v>
       </c>
@@ -2608,7 +2641,7 @@
       </c>
     </row>
     <row r="86" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A86" s="9" t="s">
+      <c r="A86" s="10" t="s">
         <v>174</v>
       </c>
       <c r="B86" s="1" t="s">
@@ -2628,7 +2661,7 @@
       </c>
     </row>
     <row r="87" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A87" s="9"/>
+      <c r="A87" s="10"/>
       <c r="B87" s="1" t="s">
         <v>97</v>
       </c>
@@ -2646,7 +2679,7 @@
       </c>
     </row>
     <row r="88" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A88" s="9" t="s">
+      <c r="A88" s="10" t="s">
         <v>116</v>
       </c>
       <c r="B88" s="1" t="s">
@@ -2666,7 +2699,7 @@
       </c>
     </row>
     <row r="89" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A89" s="9"/>
+      <c r="A89" s="10"/>
       <c r="B89" s="1" t="s">
         <v>97</v>
       </c>
@@ -2684,7 +2717,7 @@
       </c>
     </row>
     <row r="90" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A90" s="9" t="s">
+      <c r="A90" s="10" t="s">
         <v>117</v>
       </c>
       <c r="B90" s="1" t="s">
@@ -2704,7 +2737,7 @@
       </c>
     </row>
     <row r="91" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A91" s="9"/>
+      <c r="A91" s="10"/>
       <c r="B91" s="1" t="s">
         <v>97</v>
       </c>
@@ -2722,7 +2755,7 @@
       </c>
     </row>
     <row r="92" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A92" s="9" t="s">
+      <c r="A92" s="10" t="s">
         <v>118</v>
       </c>
       <c r="B92" s="1" t="s">
@@ -2742,7 +2775,7 @@
       </c>
     </row>
     <row r="93" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A93" s="9"/>
+      <c r="A93" s="10"/>
       <c r="B93" s="1" t="s">
         <v>97</v>
       </c>
@@ -2760,7 +2793,7 @@
       </c>
     </row>
     <row r="94" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A94" s="9" t="s">
+      <c r="A94" s="10" t="s">
         <v>119</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -2780,7 +2813,7 @@
       </c>
     </row>
     <row r="95" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A95" s="9"/>
+      <c r="A95" s="10"/>
       <c r="B95" s="1" t="s">
         <v>97</v>
       </c>
@@ -2798,7 +2831,7 @@
       </c>
     </row>
     <row r="96" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A96" s="9" t="s">
+      <c r="A96" s="10" t="s">
         <v>120</v>
       </c>
       <c r="B96" s="1" t="s">
@@ -2818,7 +2851,7 @@
       </c>
     </row>
     <row r="97" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A97" s="9"/>
+      <c r="A97" s="10"/>
       <c r="B97" s="1" t="s">
         <v>97</v>
       </c>
@@ -2870,15 +2903,15 @@
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A100" s="9"/>
-      <c r="B100" s="9"/>
-      <c r="C100" s="9"/>
-      <c r="D100" s="9"/>
-      <c r="E100" s="9"/>
-      <c r="F100" s="9"/>
+      <c r="A100" s="10"/>
+      <c r="B100" s="10"/>
+      <c r="C100" s="10"/>
+      <c r="D100" s="10"/>
+      <c r="E100" s="10"/>
+      <c r="F100" s="10"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A101" s="9" t="s">
+      <c r="A101" s="10" t="s">
         <v>124</v>
       </c>
       <c r="B101" s="1" t="s">
@@ -2895,7 +2928,7 @@
       </c>
     </row>
     <row r="102" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A102" s="9"/>
+      <c r="A102" s="10"/>
       <c r="B102" s="1" t="s">
         <v>74</v>
       </c>
@@ -2910,7 +2943,7 @@
       </c>
     </row>
     <row r="103" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A103" s="9"/>
+      <c r="A103" s="10"/>
       <c r="B103" s="1" t="s">
         <v>75</v>
       </c>
@@ -2925,7 +2958,7 @@
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A104" s="9"/>
+      <c r="A104" s="10"/>
       <c r="B104" s="1" t="s">
         <v>76</v>
       </c>
@@ -2940,7 +2973,7 @@
       </c>
     </row>
     <row r="105" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A105" s="9"/>
+      <c r="A105" s="10"/>
       <c r="B105" s="1" t="s">
         <v>77</v>
       </c>
@@ -2955,7 +2988,7 @@
       </c>
     </row>
     <row r="106" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A106" s="9"/>
+      <c r="A106" s="10"/>
       <c r="B106" s="1" t="s">
         <v>78</v>
       </c>
@@ -2970,15 +3003,15 @@
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A107" s="9"/>
-      <c r="B107" s="9"/>
-      <c r="C107" s="9"/>
-      <c r="D107" s="9"/>
-      <c r="E107" s="9"/>
-      <c r="F107" s="9"/>
+      <c r="A107" s="10"/>
+      <c r="B107" s="10"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="10"/>
+      <c r="E107" s="10"/>
+      <c r="F107" s="10"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A108" s="9" t="s">
+      <c r="A108" s="10" t="s">
         <v>131</v>
       </c>
       <c r="B108" s="1" t="s">
@@ -2998,7 +3031,7 @@
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A109" s="9"/>
+      <c r="A109" s="10"/>
       <c r="B109" s="1" t="s">
         <v>74</v>
       </c>
@@ -3016,7 +3049,7 @@
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A110" s="9"/>
+      <c r="A110" s="10"/>
       <c r="B110" s="1" t="s">
         <v>75</v>
       </c>
@@ -3034,7 +3067,7 @@
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A111" s="9"/>
+      <c r="A111" s="10"/>
       <c r="B111" s="1" t="s">
         <v>76</v>
       </c>
@@ -3052,15 +3085,15 @@
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A112" s="9"/>
-      <c r="B112" s="9"/>
-      <c r="C112" s="9"/>
-      <c r="D112" s="9"/>
-      <c r="E112" s="9"/>
-      <c r="F112" s="9"/>
+      <c r="A112" s="10"/>
+      <c r="B112" s="10"/>
+      <c r="C112" s="10"/>
+      <c r="D112" s="10"/>
+      <c r="E112" s="10"/>
+      <c r="F112" s="10"/>
     </row>
     <row r="113" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A113" s="9" t="s">
+      <c r="A113" s="10" t="s">
         <v>136</v>
       </c>
       <c r="B113" s="1" t="s">
@@ -3080,7 +3113,7 @@
       </c>
     </row>
     <row r="114" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A114" s="9"/>
+      <c r="A114" s="10"/>
       <c r="B114" s="1" t="s">
         <v>97</v>
       </c>
@@ -3098,7 +3131,7 @@
       </c>
     </row>
     <row r="115" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A115" s="9" t="s">
+      <c r="A115" s="10" t="s">
         <v>137</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -3118,7 +3151,7 @@
       </c>
     </row>
     <row r="116" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A116" s="9"/>
+      <c r="A116" s="10"/>
       <c r="B116" s="1" t="s">
         <v>97</v>
       </c>
@@ -3136,15 +3169,15 @@
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A117" s="9"/>
-      <c r="B117" s="9"/>
-      <c r="C117" s="9"/>
-      <c r="D117" s="9"/>
-      <c r="E117" s="9"/>
-      <c r="F117" s="9"/>
+      <c r="A117" s="10"/>
+      <c r="B117" s="10"/>
+      <c r="C117" s="10"/>
+      <c r="D117" s="10"/>
+      <c r="E117" s="10"/>
+      <c r="F117" s="10"/>
     </row>
     <row r="118" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A118" s="9" t="s">
+      <c r="A118" s="10" t="s">
         <v>141</v>
       </c>
       <c r="B118" s="1" t="s">
@@ -3164,7 +3197,7 @@
       </c>
     </row>
     <row r="119" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A119" s="9"/>
+      <c r="A119" s="10"/>
       <c r="B119" s="1" t="s">
         <v>158</v>
       </c>
@@ -3182,15 +3215,15 @@
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A120" s="9"/>
-      <c r="B120" s="9"/>
-      <c r="C120" s="9"/>
-      <c r="D120" s="9"/>
-      <c r="E120" s="9"/>
-      <c r="F120" s="9"/>
+      <c r="A120" s="10"/>
+      <c r="B120" s="10"/>
+      <c r="C120" s="10"/>
+      <c r="D120" s="10"/>
+      <c r="E120" s="10"/>
+      <c r="F120" s="10"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A121" s="9" t="s">
+      <c r="A121" s="10" t="s">
         <v>142</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -3207,7 +3240,7 @@
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A122" s="9"/>
+      <c r="A122" s="10"/>
       <c r="B122" s="1" t="s">
         <v>74</v>
       </c>
@@ -3222,15 +3255,15 @@
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A123" s="9"/>
-      <c r="B123" s="9"/>
-      <c r="C123" s="9"/>
-      <c r="D123" s="9"/>
-      <c r="E123" s="9"/>
-      <c r="F123" s="9"/>
+      <c r="A123" s="10"/>
+      <c r="B123" s="10"/>
+      <c r="C123" s="10"/>
+      <c r="D123" s="10"/>
+      <c r="E123" s="10"/>
+      <c r="F123" s="10"/>
     </row>
     <row r="124" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A124" s="9" t="s">
+      <c r="A124" s="10" t="s">
         <v>176</v>
       </c>
       <c r="B124" s="1" t="s">
@@ -3247,7 +3280,7 @@
       </c>
     </row>
     <row r="125" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A125" s="9"/>
+      <c r="A125" s="10"/>
       <c r="B125" s="6" t="s">
         <v>74</v>
       </c>
@@ -3262,7 +3295,7 @@
       </c>
     </row>
     <row r="126" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A126" s="9"/>
+      <c r="A126" s="10"/>
       <c r="B126" s="6" t="s">
         <v>75</v>
       </c>
@@ -3276,50 +3309,110 @@
         <v>183</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A128" s="1" t="s">
+    <row r="127" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A127" s="10"/>
+      <c r="B127" s="11"/>
+      <c r="C127" s="11"/>
+      <c r="D127" s="11"/>
+      <c r="E127" s="11"/>
+      <c r="F127" s="11"/>
+    </row>
+    <row r="128" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A128" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="B128" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="C128" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="D128" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="E128" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="F128" s="12" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A129" s="10"/>
+      <c r="B129" s="11"/>
+      <c r="C129" s="11"/>
+      <c r="D129" s="11"/>
+      <c r="E129" s="11"/>
+      <c r="F129" s="11"/>
+    </row>
+    <row r="130" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A130" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="B130" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C128" s="1" t="s">
+      <c r="C130" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E128" s="4" t="s">
+      <c r="E130" s="4" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="27" x14ac:dyDescent="0.15">
-      <c r="A129" s="7" t="s">
+    <row r="131" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A131" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="B129" s="7" t="s">
+      <c r="B131" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="C129" s="1" t="s">
+      <c r="C131" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E129" s="4" t="s">
+      <c r="E131" s="4" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A130" s="7" t="s">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A132" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="B130" s="7" t="s">
+      <c r="B132" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="C130" s="1" t="s">
+      <c r="C132" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="E130" s="2" t="s">
+      <c r="E132" s="2" t="s">
         <v>206</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="38">
+  <mergeCells count="40">
+    <mergeCell ref="A127:F127"/>
+    <mergeCell ref="A129:F129"/>
+    <mergeCell ref="A112:F112"/>
+    <mergeCell ref="A124:A126"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="A121:A122"/>
+    <mergeCell ref="A113:A114"/>
+    <mergeCell ref="A115:A116"/>
+    <mergeCell ref="A123:F123"/>
+    <mergeCell ref="A120:F120"/>
+    <mergeCell ref="A117:F117"/>
+    <mergeCell ref="A100:F100"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="A26:A33"/>
+    <mergeCell ref="A34:A41"/>
+    <mergeCell ref="A51:A58"/>
+    <mergeCell ref="A59:A66"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="A50:F50"/>
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="A83:F83"/>
+    <mergeCell ref="A67:F67"/>
     <mergeCell ref="A101:A106"/>
     <mergeCell ref="A108:A111"/>
     <mergeCell ref="A68:A69"/>
@@ -3336,28 +3429,6 @@
     <mergeCell ref="A94:A95"/>
     <mergeCell ref="A96:A97"/>
     <mergeCell ref="A107:F107"/>
-    <mergeCell ref="A100:F100"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A10:A17"/>
-    <mergeCell ref="A18:A25"/>
-    <mergeCell ref="A26:A33"/>
-    <mergeCell ref="A34:A41"/>
-    <mergeCell ref="A51:A58"/>
-    <mergeCell ref="A59:A66"/>
-    <mergeCell ref="A42:A49"/>
-    <mergeCell ref="A50:F50"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="A83:F83"/>
-    <mergeCell ref="A67:F67"/>
-    <mergeCell ref="A112:F112"/>
-    <mergeCell ref="A124:A126"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="A121:A122"/>
-    <mergeCell ref="A113:A114"/>
-    <mergeCell ref="A115:A116"/>
-    <mergeCell ref="A123:F123"/>
-    <mergeCell ref="A120:F120"/>
-    <mergeCell ref="A117:F117"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update spec to V0.5
</commit_message>
<xml_diff>
--- a/DOC/register map.xlsx
+++ b/DOC/register map.xlsx
@@ -253,10 +253,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>HDD 12V/5V Power Enable</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Field</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -869,6 +865,11 @@
   <si>
     <t>0</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDD 12V/5V Power Enable
+When this bit is 0, the PWR_EN_HDD1 will be set to high</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -959,19 +960,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1255,8 +1256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="A128" sqref="A128:F128"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1275,7 +1276,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>1</v>
@@ -1291,27 +1292,27 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="7" t="s">
-        <v>81</v>
+      <c r="A2" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="7"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>3</v>
@@ -1319,15 +1320,15 @@
       <c r="D3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="7"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>4</v>
@@ -1335,15 +1336,15 @@
       <c r="D4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="7"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>5</v>
@@ -1351,15 +1352,15 @@
       <c r="D5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="7"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>6</v>
@@ -1367,15 +1368,15 @@
       <c r="D6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="7"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>7</v>
@@ -1383,15 +1384,15 @@
       <c r="D7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" s="7"/>
+      <c r="A8" s="10"/>
       <c r="B8" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>8</v>
@@ -1399,15 +1400,15 @@
       <c r="D8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9" s="7"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>9</v>
@@ -1415,17 +1416,17 @@
       <c r="D9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="7" t="s">
-        <v>162</v>
+      <c r="A10" s="10" t="s">
+        <v>161</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>10</v>
@@ -1433,15 +1434,15 @@
       <c r="D10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="7"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>11</v>
@@ -1449,15 +1450,15 @@
       <c r="D11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="7"/>
+      <c r="A12" s="10"/>
       <c r="B12" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>12</v>
@@ -1465,15 +1466,15 @@
       <c r="D12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="7"/>
+      <c r="A13" s="10"/>
       <c r="B13" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>13</v>
@@ -1481,15 +1482,15 @@
       <c r="D13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="7"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>14</v>
@@ -1497,15 +1498,15 @@
       <c r="D14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="7"/>
+      <c r="A15" s="10"/>
       <c r="B15" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>15</v>
@@ -1513,15 +1514,15 @@
       <c r="D15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="7"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>16</v>
@@ -1529,31 +1530,31 @@
       <c r="D16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A17" s="7"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>192</v>
-      </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="8" t="s">
-        <v>194</v>
+      <c r="E17" s="7" t="s">
+        <v>193</v>
       </c>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A18" s="7" t="s">
-        <v>163</v>
+      <c r="A18" s="10" t="s">
+        <v>162</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>21</v>
@@ -1561,15 +1562,15 @@
       <c r="D18" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="7" t="s">
         <v>38</v>
       </c>
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A19" s="7"/>
+      <c r="A19" s="10"/>
       <c r="B19" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>22</v>
@@ -1577,15 +1578,15 @@
       <c r="D19" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="7" t="s">
         <v>38</v>
       </c>
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A20" s="7"/>
+      <c r="A20" s="10"/>
       <c r="B20" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>23</v>
@@ -1593,15 +1594,15 @@
       <c r="D20" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="7" t="s">
         <v>37</v>
       </c>
       <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A21" s="7"/>
+      <c r="A21" s="10"/>
       <c r="B21" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>24</v>
@@ -1609,15 +1610,15 @@
       <c r="D21" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="7" t="s">
         <v>37</v>
       </c>
       <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A22" s="7"/>
+      <c r="A22" s="10"/>
       <c r="B22" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>25</v>
@@ -1625,15 +1626,15 @@
       <c r="D22" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="7" t="s">
         <v>37</v>
       </c>
       <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A23" s="7"/>
+      <c r="A23" s="10"/>
       <c r="B23" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>26</v>
@@ -1641,15 +1642,15 @@
       <c r="D23" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="7" t="s">
         <v>37</v>
       </c>
       <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A24" s="7"/>
+      <c r="A24" s="10"/>
       <c r="B24" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>27</v>
@@ -1657,15 +1658,15 @@
       <c r="D24" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="7" t="s">
         <v>37</v>
       </c>
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A25" s="7"/>
+      <c r="A25" s="10"/>
       <c r="B25" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>28</v>
@@ -1673,17 +1674,17 @@
       <c r="D25" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="7" t="s">
         <v>37</v>
       </c>
       <c r="F25" s="6"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A26" s="7" t="s">
-        <v>164</v>
+      <c r="A26" s="10" t="s">
+        <v>163</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>29</v>
@@ -1691,15 +1692,15 @@
       <c r="D26" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="7" t="s">
         <v>37</v>
       </c>
       <c r="F26" s="6"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A27" s="7"/>
+      <c r="A27" s="10"/>
       <c r="B27" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>30</v>
@@ -1707,15 +1708,15 @@
       <c r="D27" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="7" t="s">
         <v>37</v>
       </c>
       <c r="F27" s="6"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A28" s="7"/>
+      <c r="A28" s="10"/>
       <c r="B28" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>31</v>
@@ -1723,15 +1724,15 @@
       <c r="D28" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="7" t="s">
         <v>37</v>
       </c>
       <c r="F28" s="6"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A29" s="7"/>
+      <c r="A29" s="10"/>
       <c r="B29" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>32</v>
@@ -1739,15 +1740,15 @@
       <c r="D29" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="7" t="s">
         <v>37</v>
       </c>
       <c r="F29" s="6"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A30" s="7"/>
+      <c r="A30" s="10"/>
       <c r="B30" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>33</v>
@@ -1755,15 +1756,15 @@
       <c r="D30" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="7" t="s">
         <v>37</v>
       </c>
       <c r="F30" s="6"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A31" s="7"/>
+      <c r="A31" s="10"/>
       <c r="B31" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>34</v>
@@ -1771,15 +1772,15 @@
       <c r="D31" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="7" t="s">
         <v>37</v>
       </c>
       <c r="F31" s="6"/>
     </row>
     <row r="32" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="7"/>
+      <c r="A32" s="10"/>
       <c r="B32" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>35</v>
@@ -1787,31 +1788,31 @@
       <c r="D32" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="7" t="s">
         <v>37</v>
       </c>
       <c r="F32" s="6"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A33" s="7"/>
+      <c r="A33" s="10"/>
       <c r="B33" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D33" s="6"/>
-      <c r="E33" s="8" t="s">
-        <v>192</v>
+      <c r="E33" s="7" t="s">
+        <v>191</v>
       </c>
       <c r="F33" s="6"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A34" s="7" t="s">
-        <v>166</v>
+      <c r="A34" s="10" t="s">
+        <v>165</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>39</v>
@@ -1819,15 +1820,15 @@
       <c r="D34" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="7" t="s">
         <v>55</v>
       </c>
       <c r="F34" s="6"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A35" s="7"/>
+      <c r="A35" s="10"/>
       <c r="B35" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>40</v>
@@ -1835,15 +1836,15 @@
       <c r="D35" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="7" t="s">
         <v>55</v>
       </c>
       <c r="F35" s="6"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A36" s="7"/>
+      <c r="A36" s="10"/>
       <c r="B36" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>41</v>
@@ -1851,15 +1852,15 @@
       <c r="D36" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E36" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F36" s="6"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A37" s="7"/>
+      <c r="A37" s="10"/>
       <c r="B37" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>42</v>
@@ -1867,15 +1868,15 @@
       <c r="D37" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E37" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F37" s="6"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A38" s="7"/>
+      <c r="A38" s="10"/>
       <c r="B38" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>43</v>
@@ -1883,15 +1884,15 @@
       <c r="D38" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="E38" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F38" s="6"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A39" s="7"/>
+      <c r="A39" s="10"/>
       <c r="B39" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>44</v>
@@ -1899,15 +1900,15 @@
       <c r="D39" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="E39" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F39" s="6"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A40" s="7"/>
+      <c r="A40" s="10"/>
       <c r="B40" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>45</v>
@@ -1915,15 +1916,15 @@
       <c r="D40" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="E40" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F40" s="6"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A41" s="7"/>
+      <c r="A41" s="10"/>
       <c r="B41" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>46</v>
@@ -1931,17 +1932,17 @@
       <c r="D41" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="E41" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F41" s="6"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A42" s="7" t="s">
-        <v>165</v>
+      <c r="A42" s="10" t="s">
+        <v>164</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>47</v>
@@ -1949,15 +1950,15 @@
       <c r="D42" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="E42" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F42" s="6"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A43" s="7"/>
+      <c r="A43" s="10"/>
       <c r="B43" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>48</v>
@@ -1965,15 +1966,15 @@
       <c r="D43" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E43" s="8" t="s">
+      <c r="E43" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F43" s="6"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A44" s="7"/>
+      <c r="A44" s="10"/>
       <c r="B44" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>49</v>
@@ -1981,15 +1982,15 @@
       <c r="D44" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E44" s="8" t="s">
+      <c r="E44" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F44" s="6"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A45" s="7"/>
+      <c r="A45" s="10"/>
       <c r="B45" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>50</v>
@@ -1997,15 +1998,15 @@
       <c r="D45" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E45" s="8" t="s">
+      <c r="E45" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F45" s="6"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A46" s="7"/>
+      <c r="A46" s="10"/>
       <c r="B46" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>51</v>
@@ -2013,15 +2014,15 @@
       <c r="D46" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E46" s="8" t="s">
+      <c r="E46" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F46" s="6"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A47" s="7"/>
+      <c r="A47" s="10"/>
       <c r="B47" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>52</v>
@@ -2029,15 +2030,15 @@
       <c r="D47" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E47" s="8" t="s">
+      <c r="E47" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F47" s="6"/>
     </row>
     <row r="48" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="7"/>
+      <c r="A48" s="10"/>
       <c r="B48" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>53</v>
@@ -2045,57 +2046,57 @@
       <c r="D48" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E48" s="8" t="s">
+      <c r="E48" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F48" s="6"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A49" s="7"/>
+      <c r="A49" s="10"/>
       <c r="B49" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D49" s="6"/>
-      <c r="E49" s="8" t="s">
-        <v>192</v>
+      <c r="E49" s="7" t="s">
+        <v>191</v>
       </c>
       <c r="F49" s="6"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A51" s="7" t="s">
-        <v>82</v>
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+    </row>
+    <row r="51" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A51" s="10" t="s">
+        <v>81</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>70</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>71</v>
+        <v>232</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A52" s="7"/>
+      <c r="A52" s="10"/>
       <c r="B52" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>56</v>
@@ -2103,17 +2104,17 @@
       <c r="D52" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E52" s="8" t="s">
-        <v>161</v>
+      <c r="E52" s="7" t="s">
+        <v>160</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A53" s="7"/>
+      <c r="A53" s="10"/>
       <c r="B53" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>57</v>
@@ -2121,17 +2122,17 @@
       <c r="D53" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E53" s="8" t="s">
-        <v>160</v>
+      <c r="E53" s="7" t="s">
+        <v>159</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A54" s="7"/>
+      <c r="A54" s="10"/>
       <c r="B54" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>58</v>
@@ -2139,17 +2140,17 @@
       <c r="D54" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E54" s="8" t="s">
-        <v>160</v>
+      <c r="E54" s="7" t="s">
+        <v>159</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A55" s="7"/>
+      <c r="A55" s="10"/>
       <c r="B55" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>59</v>
@@ -2157,17 +2158,17 @@
       <c r="D55" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E55" s="8" t="s">
-        <v>160</v>
+      <c r="E55" s="7" t="s">
+        <v>159</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A56" s="7"/>
+      <c r="A56" s="10"/>
       <c r="B56" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>60</v>
@@ -2175,17 +2176,17 @@
       <c r="D56" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E56" s="8" t="s">
-        <v>160</v>
+      <c r="E56" s="7" t="s">
+        <v>159</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A57" s="7"/>
+      <c r="A57" s="10"/>
       <c r="B57" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>61</v>
@@ -2193,17 +2194,17 @@
       <c r="D57" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E57" s="8" t="s">
-        <v>160</v>
+      <c r="E57" s="7" t="s">
+        <v>159</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A58" s="7"/>
+      <c r="A58" s="10"/>
       <c r="B58" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>62</v>
@@ -2211,19 +2212,19 @@
       <c r="D58" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E58" s="8" t="s">
-        <v>160</v>
+      <c r="E58" s="7" t="s">
+        <v>159</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A59" s="7" t="s">
-        <v>159</v>
+      <c r="A59" s="10" t="s">
+        <v>158</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>63</v>
@@ -2231,17 +2232,17 @@
       <c r="D59" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E59" s="8" t="s">
-        <v>160</v>
+      <c r="E59" s="7" t="s">
+        <v>159</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A60" s="7"/>
+      <c r="A60" s="10"/>
       <c r="B60" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>64</v>
@@ -2249,17 +2250,17 @@
       <c r="D60" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E60" s="8" t="s">
-        <v>160</v>
+      <c r="E60" s="7" t="s">
+        <v>159</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A61" s="7"/>
+      <c r="A61" s="10"/>
       <c r="B61" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>65</v>
@@ -2267,17 +2268,17 @@
       <c r="D61" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E61" s="8" t="s">
-        <v>160</v>
+      <c r="E61" s="7" t="s">
+        <v>159</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A62" s="7"/>
+      <c r="A62" s="10"/>
       <c r="B62" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>66</v>
@@ -2285,17 +2286,17 @@
       <c r="D62" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E62" s="8" t="s">
-        <v>160</v>
+      <c r="E62" s="7" t="s">
+        <v>159</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A63" s="7"/>
+      <c r="A63" s="10"/>
       <c r="B63" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>67</v>
@@ -2303,17 +2304,17 @@
       <c r="D63" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E63" s="8" t="s">
-        <v>160</v>
+      <c r="E63" s="7" t="s">
+        <v>159</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A64" s="7"/>
+      <c r="A64" s="10"/>
       <c r="B64" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C64" s="6" t="s">
         <v>68</v>
@@ -2321,17 +2322,17 @@
       <c r="D64" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E64" s="8" t="s">
-        <v>160</v>
+      <c r="E64" s="7" t="s">
+        <v>159</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="65" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="7"/>
+      <c r="A65" s="10"/>
       <c r="B65" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>69</v>
@@ -2339,1161 +2340,1137 @@
       <c r="D65" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E65" s="8" t="s">
-        <v>160</v>
+      <c r="E65" s="7" t="s">
+        <v>159</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A66" s="7"/>
+      <c r="A66" s="10"/>
       <c r="B66" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D66" s="6"/>
-      <c r="E66" s="8" t="s">
-        <v>192</v>
+      <c r="E66" s="7" t="s">
+        <v>191</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A67" s="7"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="7"/>
-      <c r="D67" s="7"/>
-      <c r="E67" s="7"/>
-      <c r="F67" s="7"/>
+      <c r="A67" s="10"/>
+      <c r="B67" s="10"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="10"/>
     </row>
     <row r="68" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A68" s="7" t="s">
-        <v>98</v>
+      <c r="A68" s="10" t="s">
+        <v>97</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E68" s="9" t="s">
-        <v>99</v>
+      <c r="E68" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A69" s="7"/>
+      <c r="A69" s="10"/>
       <c r="B69" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E69" s="9" t="s">
-        <v>99</v>
+      <c r="E69" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A70" s="7" t="s">
-        <v>167</v>
+      <c r="A70" s="10" t="s">
+        <v>166</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E70" s="9" t="s">
-        <v>99</v>
+      <c r="E70" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A71" s="7"/>
+      <c r="A71" s="10"/>
       <c r="B71" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E71" s="9" t="s">
-        <v>99</v>
+      <c r="E71" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A72" s="7" t="s">
-        <v>168</v>
+      <c r="A72" s="10" t="s">
+        <v>167</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E72" s="9" t="s">
-        <v>99</v>
+      <c r="E72" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A73" s="7"/>
+      <c r="A73" s="10"/>
       <c r="B73" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E73" s="9" t="s">
-        <v>99</v>
+      <c r="E73" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A74" s="7" t="s">
-        <v>169</v>
+      <c r="A74" s="10" t="s">
+        <v>168</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E74" s="9" t="s">
-        <v>99</v>
+      <c r="E74" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A75" s="7"/>
+      <c r="A75" s="10"/>
       <c r="B75" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E75" s="9" t="s">
-        <v>99</v>
+      <c r="E75" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A76" s="7" t="s">
-        <v>170</v>
+      <c r="A76" s="10" t="s">
+        <v>169</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E76" s="9" t="s">
-        <v>99</v>
+      <c r="E76" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A77" s="7"/>
+      <c r="A77" s="10"/>
       <c r="B77" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D77" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E77" s="9" t="s">
-        <v>99</v>
+      <c r="E77" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A78" s="7" t="s">
-        <v>171</v>
+      <c r="A78" s="10" t="s">
+        <v>170</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E78" s="9" t="s">
-        <v>99</v>
+      <c r="E78" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A79" s="7"/>
+      <c r="A79" s="10"/>
       <c r="B79" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D79" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E79" s="9" t="s">
-        <v>99</v>
+      <c r="E79" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A80" s="7" t="s">
-        <v>172</v>
+      <c r="A80" s="10" t="s">
+        <v>171</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E80" s="9" t="s">
-        <v>99</v>
+      <c r="E80" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A81" s="7"/>
+      <c r="A81" s="10"/>
       <c r="B81" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E81" s="9" t="s">
-        <v>99</v>
+      <c r="E81" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="27" x14ac:dyDescent="0.15">
       <c r="A82" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E82" s="9" t="s">
+      <c r="E82" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A83" s="10"/>
+      <c r="B83" s="10"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="10"/>
+      <c r="E83" s="10"/>
+      <c r="F83" s="10"/>
+    </row>
+    <row r="84" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A84" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F82" s="6" t="s">
+      <c r="B84" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E84" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F84" s="6" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A83" s="7"/>
-      <c r="B83" s="7"/>
-      <c r="C83" s="7"/>
-      <c r="D83" s="7"/>
-      <c r="E83" s="7"/>
-      <c r="F83" s="7"/>
-    </row>
-    <row r="84" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A84" s="7" t="s">
+    <row r="85" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A85" s="10"/>
+      <c r="B85" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C85" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B84" s="6" t="s">
+      <c r="D85" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E85" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A86" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E86" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A87" s="10"/>
+      <c r="B87" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C84" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="D84" s="6" t="s">
+      <c r="C87" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E87" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A88" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="E84" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="F84" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A85" s="7"/>
-      <c r="B85" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D85" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E85" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="F85" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A86" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="B86" s="6" t="s">
+      <c r="B88" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E88" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F88" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A89" s="10"/>
+      <c r="B89" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C86" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D86" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E86" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="F86" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A87" s="7"/>
-      <c r="B87" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D87" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E87" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="F87" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A88" s="7" t="s">
+      <c r="C89" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E89" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F89" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A90" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="B88" s="6" t="s">
+      <c r="B90" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E90" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F90" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A91" s="10"/>
+      <c r="B91" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C88" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D88" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E88" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="F88" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A89" s="7"/>
-      <c r="B89" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C89" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D89" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E89" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="F89" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A90" s="7" t="s">
+      <c r="C91" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D91" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E91" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F91" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A92" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="B90" s="6" t="s">
+      <c r="B92" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E92" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F92" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A93" s="10"/>
+      <c r="B93" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C90" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D90" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E90" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="F90" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A91" s="7"/>
-      <c r="B91" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D91" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E91" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="F91" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A92" s="7" t="s">
+      <c r="C93" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E93" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F93" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A94" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="B92" s="6" t="s">
+      <c r="B94" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D94" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E94" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F94" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A95" s="10"/>
+      <c r="B95" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C92" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D92" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E92" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="F92" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A93" s="7"/>
-      <c r="B93" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="D93" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E93" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="F93" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A94" s="7" t="s">
+      <c r="C95" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D95" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E95" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F95" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A96" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="B94" s="6" t="s">
+      <c r="B96" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D96" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E96" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F96" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A97" s="10"/>
+      <c r="B97" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C94" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D94" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E94" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="F94" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A95" s="7"/>
-      <c r="B95" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C95" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D95" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E95" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="F95" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A96" s="7" t="s">
+      <c r="C97" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D97" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E97" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="B96" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C96" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="D96" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E96" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="F96" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A97" s="7"/>
-      <c r="B97" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C97" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D97" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E97" s="9" t="s">
-        <v>121</v>
-      </c>
       <c r="F97" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="98" spans="1:6" s="4" customFormat="1" ht="27" x14ac:dyDescent="0.15">
       <c r="A98" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C98" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D98" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="D98" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E98" s="9" t="s">
-        <v>121</v>
+      <c r="E98" s="8" t="s">
+        <v>120</v>
       </c>
       <c r="F98" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A99" s="6"/>
       <c r="B99" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D99" s="6"/>
-      <c r="E99" s="8" t="s">
-        <v>197</v>
+      <c r="E99" s="7" t="s">
+        <v>196</v>
       </c>
       <c r="F99" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A100" s="10"/>
+      <c r="B100" s="10"/>
+      <c r="C100" s="10"/>
+      <c r="D100" s="10"/>
+      <c r="E100" s="10"/>
+      <c r="F100" s="10"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A101" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D101" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E101" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="F101" s="6"/>
+    </row>
+    <row r="102" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A102" s="10"/>
+      <c r="B102" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C102" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D102" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E102" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="F102" s="6"/>
+    </row>
+    <row r="103" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A103" s="10"/>
+      <c r="B103" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C103" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D103" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E103" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="F103" s="6"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A104" s="10"/>
+      <c r="B104" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C104" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D104" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E104" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="F104" s="6"/>
+    </row>
+    <row r="105" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A105" s="10"/>
+      <c r="B105" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E105" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="F105" s="6"/>
+    </row>
+    <row r="106" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A106" s="10"/>
+      <c r="B106" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C106" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D106" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E106" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="F106" s="6"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A107" s="10"/>
+      <c r="B107" s="10"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="10"/>
+      <c r="E107" s="10"/>
+      <c r="F107" s="10"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A108" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B108" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C108" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D108" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E108" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="F108" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A109" s="10"/>
+      <c r="B109" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C109" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D109" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E109" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F109" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A110" s="10"/>
+      <c r="B110" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C110" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D110" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E110" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="F110" s="6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A111" s="10"/>
+      <c r="B111" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C111" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E111" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="F111" s="6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A112" s="10"/>
+      <c r="B112" s="10"/>
+      <c r="C112" s="10"/>
+      <c r="D112" s="10"/>
+      <c r="E112" s="10"/>
+      <c r="F112" s="10"/>
+    </row>
+    <row r="113" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A113" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E113" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="F113" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A114" s="10"/>
+      <c r="B114" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C114" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D114" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E114" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="F114" s="6" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A100" s="7"/>
-      <c r="B100" s="7"/>
-      <c r="C100" s="7"/>
-      <c r="D100" s="7"/>
-      <c r="E100" s="7"/>
-      <c r="F100" s="7"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A101" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="B101" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="C101" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="D101" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E101" s="8" t="s">
+    <row r="115" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A115" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C115" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="D115" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E115" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="F115" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A116" s="10"/>
+      <c r="B116" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C116" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D116" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E116" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="F116" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A117" s="10"/>
+      <c r="B117" s="10"/>
+      <c r="C117" s="10"/>
+      <c r="D117" s="10"/>
+      <c r="E117" s="10"/>
+      <c r="F117" s="10"/>
+    </row>
+    <row r="118" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A118" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B118" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D118" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E118" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="F118" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A119" s="10"/>
+      <c r="B119" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C119" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="D119" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E119" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="F119" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A120" s="10"/>
+      <c r="B120" s="10"/>
+      <c r="C120" s="10"/>
+      <c r="D120" s="10"/>
+      <c r="E120" s="10"/>
+      <c r="F120" s="10"/>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A121" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B121" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C121" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="D121" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E121" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F121" s="6"/>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A122" s="10"/>
+      <c r="B122" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C122" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D122" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E122" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F122" s="6"/>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A123" s="10"/>
+      <c r="B123" s="10"/>
+      <c r="C123" s="10"/>
+      <c r="D123" s="10"/>
+      <c r="E123" s="10"/>
+      <c r="F123" s="10"/>
+    </row>
+    <row r="124" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A124" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B124" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C124" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D124" s="6"/>
+      <c r="E124" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="F101" s="6"/>
-    </row>
-    <row r="102" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A102" s="7"/>
-      <c r="B102" s="6" t="s">
+      <c r="F124" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A125" s="10"/>
+      <c r="B125" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C125" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="D125" s="6"/>
+      <c r="E125" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="F125" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A126" s="10"/>
+      <c r="B126" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C102" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D102" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E102" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F102" s="6"/>
-    </row>
-    <row r="103" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A103" s="7"/>
-      <c r="B103" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C103" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="D103" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E103" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="F103" s="6"/>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A104" s="7"/>
-      <c r="B104" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C104" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="D104" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E104" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="F104" s="6"/>
-    </row>
-    <row r="105" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A105" s="7"/>
-      <c r="B105" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C105" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="D105" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E105" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="F105" s="6"/>
-    </row>
-    <row r="106" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A106" s="7"/>
-      <c r="B106" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C106" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="D106" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E106" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="F106" s="6"/>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A107" s="7"/>
-      <c r="B107" s="7"/>
-      <c r="C107" s="7"/>
-      <c r="D107" s="7"/>
-      <c r="E107" s="7"/>
-      <c r="F107" s="7"/>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A108" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B108" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="C108" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D108" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E108" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="F108" s="6" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A109" s="7"/>
-      <c r="B109" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C109" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="D109" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E109" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F109" s="6" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A110" s="7"/>
-      <c r="B110" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C110" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="D110" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E110" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="F110" s="6" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A111" s="7"/>
-      <c r="B111" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C111" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="D111" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E111" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F111" s="6" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A112" s="7"/>
-      <c r="B112" s="7"/>
-      <c r="C112" s="7"/>
-      <c r="D112" s="7"/>
-      <c r="E112" s="7"/>
-      <c r="F112" s="7"/>
-    </row>
-    <row r="113" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A113" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B113" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C113" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="D113" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E113" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="F113" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A114" s="7"/>
-      <c r="B114" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C114" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="D114" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E114" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="F114" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A115" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="B115" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C115" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="D115" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E115" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="F115" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A116" s="7"/>
-      <c r="B116" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C116" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D116" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E116" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="F116" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A117" s="7"/>
-      <c r="B117" s="7"/>
-      <c r="C117" s="7"/>
-      <c r="D117" s="7"/>
-      <c r="E117" s="7"/>
-      <c r="F117" s="7"/>
-    </row>
-    <row r="118" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A118" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="B118" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="C118" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="D118" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E118" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="F118" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A119" s="7"/>
-      <c r="B119" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="C119" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="D119" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E119" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="F119" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A120" s="7"/>
-      <c r="B120" s="7"/>
-      <c r="C120" s="7"/>
-      <c r="D120" s="7"/>
-      <c r="E120" s="7"/>
-      <c r="F120" s="7"/>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A121" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="B121" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="C121" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="D121" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="E121" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="F121" s="6"/>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A122" s="7"/>
-      <c r="B122" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C122" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="D122" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="E122" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="F122" s="6"/>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A123" s="7"/>
-      <c r="B123" s="7"/>
-      <c r="C123" s="7"/>
-      <c r="D123" s="7"/>
-      <c r="E123" s="7"/>
-      <c r="F123" s="7"/>
-    </row>
-    <row r="124" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A124" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="B124" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="C124" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="D124" s="6"/>
-      <c r="E124" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="F124" s="6" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A125" s="7"/>
-      <c r="B125" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C125" s="6" t="s">
+      <c r="C126" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="D125" s="6"/>
-      <c r="E125" s="9" t="s">
+      <c r="D126" s="6"/>
+      <c r="E126" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="F125" s="6" t="s">
+      <c r="F126" s="6" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="A126" s="7"/>
-      <c r="B126" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C126" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="D126" s="6"/>
-      <c r="E126" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="F126" s="6" t="s">
-        <v>183</v>
-      </c>
-    </row>
     <row r="127" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A127" s="7"/>
-      <c r="B127" s="10"/>
-      <c r="C127" s="10"/>
-      <c r="D127" s="10"/>
-      <c r="E127" s="10"/>
-      <c r="F127" s="10"/>
+      <c r="A127" s="10"/>
+      <c r="B127" s="11"/>
+      <c r="C127" s="11"/>
+      <c r="D127" s="11"/>
+      <c r="E127" s="11"/>
+      <c r="F127" s="11"/>
     </row>
     <row r="128" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A128" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="B128" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="B128" s="6" t="s">
+      <c r="C128" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="C128" s="6" t="s">
+      <c r="D128" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="D128" s="6" t="s">
+      <c r="E128" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="E128" s="9" t="s">
+      <c r="F128" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="F128" s="11" t="s">
-        <v>232</v>
-      </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A129" s="7"/>
-      <c r="B129" s="10"/>
-      <c r="C129" s="10"/>
-      <c r="D129" s="10"/>
-      <c r="E129" s="10"/>
-      <c r="F129" s="10"/>
+      <c r="A129" s="10"/>
+      <c r="B129" s="11"/>
+      <c r="C129" s="11"/>
+      <c r="D129" s="11"/>
+      <c r="E129" s="11"/>
+      <c r="F129" s="11"/>
     </row>
     <row r="130" spans="1:6" ht="27" x14ac:dyDescent="0.15">
       <c r="A130" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B130" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="C130" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="C130" s="6" t="s">
-        <v>199</v>
-      </c>
       <c r="D130" s="6"/>
-      <c r="E130" s="9" t="s">
-        <v>205</v>
+      <c r="E130" s="8" t="s">
+        <v>204</v>
       </c>
       <c r="F130" s="6"/>
     </row>
     <row r="131" spans="1:6" ht="27" x14ac:dyDescent="0.15">
       <c r="A131" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D131" s="6"/>
-      <c r="E131" s="9" t="s">
-        <v>204</v>
+      <c r="E131" s="8" t="s">
+        <v>203</v>
       </c>
       <c r="F131" s="6"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A132" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D132" s="6"/>
-      <c r="E132" s="8" t="s">
-        <v>206</v>
+      <c r="E132" s="7" t="s">
+        <v>205</v>
       </c>
       <c r="F132" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A127:F127"/>
-    <mergeCell ref="A129:F129"/>
-    <mergeCell ref="A112:F112"/>
-    <mergeCell ref="A124:A126"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="A121:A122"/>
-    <mergeCell ref="A113:A114"/>
-    <mergeCell ref="A115:A116"/>
-    <mergeCell ref="A123:F123"/>
-    <mergeCell ref="A120:F120"/>
-    <mergeCell ref="A117:F117"/>
-    <mergeCell ref="A100:F100"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A10:A17"/>
-    <mergeCell ref="A18:A25"/>
-    <mergeCell ref="A26:A33"/>
-    <mergeCell ref="A34:A41"/>
-    <mergeCell ref="A51:A58"/>
-    <mergeCell ref="A59:A66"/>
-    <mergeCell ref="A42:A49"/>
-    <mergeCell ref="A50:F50"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="A83:F83"/>
-    <mergeCell ref="A67:F67"/>
     <mergeCell ref="A101:A106"/>
     <mergeCell ref="A108:A111"/>
     <mergeCell ref="A68:A69"/>
@@ -3510,6 +3487,30 @@
     <mergeCell ref="A94:A95"/>
     <mergeCell ref="A96:A97"/>
     <mergeCell ref="A107:F107"/>
+    <mergeCell ref="A100:F100"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="A26:A33"/>
+    <mergeCell ref="A34:A41"/>
+    <mergeCell ref="A51:A58"/>
+    <mergeCell ref="A59:A66"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="A50:F50"/>
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="A83:F83"/>
+    <mergeCell ref="A67:F67"/>
+    <mergeCell ref="A127:F127"/>
+    <mergeCell ref="A129:F129"/>
+    <mergeCell ref="A112:F112"/>
+    <mergeCell ref="A124:A126"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="A121:A122"/>
+    <mergeCell ref="A113:A114"/>
+    <mergeCell ref="A115:A116"/>
+    <mergeCell ref="A123:F123"/>
+    <mergeCell ref="A120:F120"/>
+    <mergeCell ref="A117:F117"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>